<commit_message>
- add 50 multiproperty points from 10.1016/j.jallcom.2022.166593
</commit_message>
<xml_diff>
--- a/Compilation_HardnessAndDuctility.xlsx
+++ b/Compilation_HardnessAndDuctility.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-contribute-Detor2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8124FFAB-5916-1341-AD31-7C723C1D469C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81E0C72-6E54-4149-9BDB-40BE5D8A94F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33760" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="154">
   <si>
     <t>Name:</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>Scratch (NOT UPLOADED)</t>
-  </si>
-  <si>
-    <t>Temperature in F</t>
   </si>
   <si>
     <t>Some Notes</t>
@@ -317,9 +314,15 @@
     <t>F</t>
   </si>
   <si>
+    <t>estimated compressive ductility</t>
+  </si>
+  <si>
     <t>%</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>AC</t>
   </si>
   <si>
@@ -368,6 +371,114 @@
     <t>14</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
     <t xml:space="preserve">MoNbTaW </t>
   </si>
   <si>
@@ -377,6 +488,9 @@
     <t xml:space="preserve">MoNbTaWTi </t>
   </si>
   <si>
+    <t>AC+A</t>
+  </si>
+  <si>
     <t>48h at 1200*C</t>
   </si>
   <si>
@@ -429,6 +543,51 @@
   </si>
   <si>
     <t>10.1016/j.actamat.2023.118728</t>
+  </si>
+  <si>
+    <t>Zr Nb Ta Hf0.2</t>
+  </si>
+  <si>
+    <t>Zr Nb Ta Hf0.2 Cr0.3</t>
+  </si>
+  <si>
+    <t>Zr Nb Ta Hf0.2 Cr0.5</t>
+  </si>
+  <si>
+    <t>Zr Nb Ta Hf0.2 Cr0.75</t>
+  </si>
+  <si>
+    <t>Zr Nb Ta Hf0.2 Cr1</t>
+  </si>
+  <si>
+    <t>BCC+HCP</t>
+  </si>
+  <si>
+    <t>BCC+HCP+C15</t>
+  </si>
+  <si>
+    <t>24h at 1400*C</t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2022.166593</t>
+  </si>
+  <si>
+    <t>strenght</t>
+  </si>
+  <si>
+    <t>compressive ductility</t>
+  </si>
+  <si>
+    <t>g/cm^3</t>
+  </si>
+  <si>
+    <t>compressive yield strength</t>
+  </si>
+  <si>
+    <t>ultimate compressive strength</t>
+  </si>
+  <si>
+    <t>density</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1175,6 +1334,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1459,7 +1619,7 @@
   <dimension ref="A1:T431"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1493,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="42" t="s">
         <v>32</v>
@@ -1515,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="45"/>
@@ -1543,7 +1703,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="54" t="s">
         <v>30</v>
@@ -1555,34 +1715,34 @@
         <v>26</v>
       </c>
       <c r="F5" s="55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G5" s="55" t="s">
         <v>27</v>
       </c>
       <c r="H5" s="62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" s="55" t="s">
         <v>28</v>
       </c>
       <c r="K5" s="55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L5" s="55" t="s">
         <v>28</v>
       </c>
       <c r="M5" s="55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N5" s="55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O5" s="56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1614,22 +1774,22 @@
         <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>19</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I7" s="6">
         <v>298</v>
@@ -1638,26 +1798,26 @@
         <v>33</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="O7" s="58"/>
       <c r="P7" s="31" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="Q7" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="R7" s="23" t="s">
         <v>40</v>
-      </c>
-      <c r="R7" s="23" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1682,7 +1842,7 @@
       </c>
       <c r="N8" s="53"/>
       <c r="O8" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P8" s="59" t="s">
         <v>39</v>
@@ -1715,7 +1875,7 @@
         <v>13</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>20</v>
@@ -1724,10 +1884,10 @@
         <v>21</v>
       </c>
       <c r="K9" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L9" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M9" s="26" t="s">
         <v>15</v>
@@ -1754,20 +1914,20 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>19</v>
@@ -1782,13 +1942,13 @@
       </c>
       <c r="K10" s="32"/>
       <c r="L10" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="P10">
         <v>560</v>
@@ -1796,20 +1956,20 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G11" s="33" t="s">
         <v>19</v>
@@ -1824,13 +1984,13 @@
       </c>
       <c r="K11" s="32"/>
       <c r="L11" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="P11">
         <v>440</v>
@@ -1838,20 +1998,20 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="33" t="s">
         <v>19</v>
@@ -1866,13 +2026,13 @@
       </c>
       <c r="K12" s="32"/>
       <c r="L12" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="P12">
         <v>480</v>
@@ -1880,22 +2040,22 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="F13" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="33" t="s">
         <v>19</v>
@@ -1910,13 +2070,13 @@
       </c>
       <c r="K13" s="32"/>
       <c r="L13" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="O13" s="20"/>
       <c r="P13">
@@ -1925,22 +2085,22 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="F14" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G14" s="33" t="s">
         <v>19</v>
@@ -1955,13 +2115,13 @@
       </c>
       <c r="K14" s="32"/>
       <c r="L14" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="O14" s="20"/>
       <c r="P14">
@@ -1970,22 +2130,22 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="F15" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G15" s="33" t="s">
         <v>19</v>
@@ -2000,13 +2160,13 @@
       </c>
       <c r="K15" s="32"/>
       <c r="L15" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="O15" s="20"/>
       <c r="P15">
@@ -2015,22 +2175,22 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G16" s="33" t="s">
         <v>19</v>
@@ -2045,35 +2205,35 @@
       </c>
       <c r="K16" s="32"/>
       <c r="L16" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M16" s="20" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="N16" s="20" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="O16" s="20"/>
       <c r="P16">
         <v>480</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="33" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="G17" s="33" t="s">
         <v>19</v>
@@ -2087,33 +2247,33 @@
       </c>
       <c r="K17" s="32"/>
       <c r="L17" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="N17" s="64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="C18" s="33" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="F18" s="33" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="G18" s="33" t="s">
         <v>19</v>
@@ -2127,33 +2287,33 @@
       </c>
       <c r="K18" s="32"/>
       <c r="L18" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="N18" s="64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="F19" s="33" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="G19" s="33" t="s">
         <v>19</v>
@@ -2167,31 +2327,31 @@
       </c>
       <c r="K19" s="32"/>
       <c r="L19" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M19" s="20" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="N19" s="64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="33" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="G20" s="33" t="s">
         <v>19</v>
@@ -2208,30 +2368,30 @@
         <v>63</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="N20" s="64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="G21" s="33" t="s">
         <v>19</v>
@@ -2248,30 +2408,30 @@
         <v>63</v>
       </c>
       <c r="M21" s="20" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="N21" s="64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="G22" s="33" t="s">
         <v>19</v>
@@ -2288,742 +2448,1991 @@
         <v>63</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="N22" s="64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E23" s="20"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
+      <c r="F23" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H23" s="33"/>
       <c r="I23" s="35">
         <v>298</v>
       </c>
-      <c r="J23" s="32"/>
+      <c r="J23" s="32">
+        <f>Q23*1000000</f>
+        <v>721000000</v>
+      </c>
       <c r="K23" s="32"/>
       <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="36"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
+      <c r="M23" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N23" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q23">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E24" s="20"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
+      <c r="F24" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G24" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H24" s="33"/>
       <c r="I24" s="35">
         <v>298</v>
       </c>
-      <c r="J24" s="32"/>
+      <c r="J24" s="32">
+        <f t="shared" ref="J24:J42" si="1">Q24*1000000</f>
+        <v>855000000</v>
+      </c>
       <c r="K24" s="32"/>
       <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="36"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
+      <c r="M24" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N24" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q24">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E25" s="20"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
+      <c r="F25" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G25" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H25" s="33"/>
       <c r="I25" s="35">
         <v>298</v>
       </c>
-      <c r="J25" s="32"/>
+      <c r="J25" s="32">
+        <f t="shared" si="1"/>
+        <v>932000000</v>
+      </c>
       <c r="K25" s="32"/>
       <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="36"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
+      <c r="M25" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N25" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q25">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E26" s="20"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
+      <c r="F26" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G26" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H26" s="33"/>
       <c r="I26" s="35">
         <v>298</v>
       </c>
-      <c r="J26" s="32"/>
+      <c r="J26" s="32">
+        <f t="shared" si="1"/>
+        <v>993000000</v>
+      </c>
       <c r="K26" s="32"/>
       <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="36"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
+      <c r="M26" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N26" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q26">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E27" s="20"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
+      <c r="F27" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H27" s="33"/>
       <c r="I27" s="35">
         <v>298</v>
       </c>
-      <c r="J27" s="32"/>
+      <c r="J27" s="32">
+        <f t="shared" si="1"/>
+        <v>1389000000</v>
+      </c>
       <c r="K27" s="32"/>
       <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="36"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
+      <c r="M27" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N27" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q27">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H28" s="33"/>
       <c r="I28" s="35">
         <v>298</v>
       </c>
-      <c r="J28" s="32"/>
+      <c r="J28" s="32">
+        <f t="shared" si="1"/>
+        <v>793000000</v>
+      </c>
       <c r="K28" s="32"/>
       <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="36"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
+      <c r="M28" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N28" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q28">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H29" s="33"/>
       <c r="I29" s="35">
         <v>298</v>
       </c>
-      <c r="J29" s="32"/>
+      <c r="J29" s="32">
+        <f t="shared" si="1"/>
+        <v>945000000</v>
+      </c>
       <c r="K29" s="32"/>
       <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="20"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="36"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
+      <c r="M29" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N29" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q29">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H30" s="33"/>
       <c r="I30" s="35">
         <v>298</v>
       </c>
-      <c r="J30" s="32"/>
+      <c r="J30" s="32">
+        <f t="shared" si="1"/>
+        <v>1021000000</v>
+      </c>
       <c r="K30" s="32"/>
       <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="36"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
+      <c r="M30" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N30" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q30">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F31" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H31" s="33"/>
       <c r="I31" s="35">
         <v>298</v>
       </c>
-      <c r="J31" s="32"/>
+      <c r="J31" s="32">
+        <f t="shared" si="1"/>
+        <v>1181000000</v>
+      </c>
       <c r="K31" s="32"/>
       <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
+      <c r="M31" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N31" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q31">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H32" s="33"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="32"/>
+      <c r="I32" s="35">
+        <v>298</v>
+      </c>
+      <c r="J32" s="32">
+        <f t="shared" si="1"/>
+        <v>1502000000</v>
+      </c>
       <c r="K32" s="32"/>
       <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="36"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="M32" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N32" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q32">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E33" s="20"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
+      <c r="F33" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H33" s="33"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="32"/>
+      <c r="I33" s="35">
+        <v>298</v>
+      </c>
+      <c r="J33" s="32">
+        <f t="shared" si="1"/>
+        <v>984000000</v>
+      </c>
       <c r="K33" s="32"/>
       <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="36"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
+      <c r="M33" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N33" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q33">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E34" s="20"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
+      <c r="F34" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G34" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H34" s="33"/>
-      <c r="I34" s="35"/>
+      <c r="I34" s="35">
+        <v>298</v>
+      </c>
+      <c r="J34" s="32">
+        <f t="shared" si="1"/>
+        <v>985000000</v>
+      </c>
       <c r="K34" s="32"/>
       <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="36"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
+      <c r="M34" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N34" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q34">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E35" s="20"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
+      <c r="F35" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H35" s="33"/>
-      <c r="I35" s="35"/>
+      <c r="I35" s="35">
+        <v>298</v>
+      </c>
+      <c r="J35" s="32">
+        <f t="shared" si="1"/>
+        <v>1025000000</v>
+      </c>
       <c r="K35" s="32"/>
       <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
+      <c r="M35" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N35" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q35">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E36" s="20"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
+      <c r="F36" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H36" s="33"/>
-      <c r="I36" s="35"/>
+      <c r="I36" s="35">
+        <v>298</v>
+      </c>
+      <c r="J36" s="32">
+        <f t="shared" si="1"/>
+        <v>1177000000</v>
+      </c>
       <c r="K36" s="32"/>
       <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
+      <c r="M36" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N36" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q36">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E37" s="20"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
+      <c r="F37" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H37" s="33"/>
-      <c r="I37" s="35"/>
+      <c r="I37" s="35">
+        <v>298</v>
+      </c>
+      <c r="J37" s="32">
+        <f t="shared" si="1"/>
+        <v>1420000000</v>
+      </c>
       <c r="K37" s="32"/>
       <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="36"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="33"/>
+      <c r="M37" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N37" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q37">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G38" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H38" s="33"/>
-      <c r="I38" s="35"/>
+      <c r="I38" s="35">
+        <v>298</v>
+      </c>
+      <c r="J38" s="32">
+        <f t="shared" si="1"/>
+        <v>1085000000</v>
+      </c>
       <c r="K38" s="32"/>
       <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="36"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="33"/>
+      <c r="M38" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N38" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q38">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F39" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H39" s="33"/>
-      <c r="I39" s="35"/>
+      <c r="I39" s="35">
+        <v>298</v>
+      </c>
+      <c r="J39" s="32">
+        <f t="shared" si="1"/>
+        <v>980000000</v>
+      </c>
       <c r="K39" s="32"/>
       <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="36"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
+      <c r="M39" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N39" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q39">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>141</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G40" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H40" s="33"/>
-      <c r="I40" s="35"/>
+      <c r="I40" s="35">
+        <v>298</v>
+      </c>
+      <c r="J40" s="32">
+        <f t="shared" si="1"/>
+        <v>1081000000</v>
+      </c>
       <c r="K40" s="32"/>
       <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
+      <c r="M40" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N40" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q40">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H41" s="33"/>
-      <c r="I41" s="35"/>
+      <c r="I41" s="35">
+        <v>298</v>
+      </c>
+      <c r="J41" s="32">
+        <f t="shared" si="1"/>
+        <v>1221000000</v>
+      </c>
       <c r="K41" s="32"/>
       <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="36"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="33"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
+      <c r="M41" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N41" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q41">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H42" s="33"/>
-      <c r="I42" s="35"/>
+      <c r="I42" s="35">
+        <v>298</v>
+      </c>
+      <c r="J42" s="32">
+        <f t="shared" si="1"/>
+        <v>1548000000</v>
+      </c>
       <c r="K42" s="32"/>
       <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="36"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
+      <c r="M42" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N42" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q42">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E43" s="20"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="35"/>
+      <c r="F43" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G43" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="35">
+        <v>298</v>
+      </c>
+      <c r="J43" s="65">
+        <v>50</v>
+      </c>
       <c r="K43" s="32"/>
       <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="36"/>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33"/>
+      <c r="M43" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N43" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E44" s="20"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="35"/>
+      <c r="F44" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G44" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="35">
+        <v>298</v>
+      </c>
+      <c r="J44" s="65">
+        <v>14.9</v>
+      </c>
       <c r="K44" s="32"/>
       <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="20"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="36"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
+      <c r="M44" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N44" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E45" s="20"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="35"/>
+      <c r="F45" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" s="35">
+        <v>298</v>
+      </c>
+      <c r="J45" s="65">
+        <v>14.2</v>
+      </c>
       <c r="K45" s="32"/>
       <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="20"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="36"/>
-      <c r="C46" s="33"/>
-      <c r="D46" s="33"/>
+      <c r="M45" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N45" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E46" s="20"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="35"/>
+      <c r="F46" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G46" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I46" s="35">
+        <v>298</v>
+      </c>
+      <c r="J46" s="65">
+        <v>12.1</v>
+      </c>
       <c r="K46" s="32"/>
       <c r="L46" s="20"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="20"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="36"/>
-      <c r="C47" s="33"/>
-      <c r="D47" s="33"/>
+      <c r="M46" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N46" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E47" s="20"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="35"/>
+      <c r="F47" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G47" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" s="35">
+        <v>298</v>
+      </c>
+      <c r="J47" s="65">
+        <v>9.1999999999999993</v>
+      </c>
       <c r="K47" s="32"/>
       <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="35"/>
+      <c r="M47" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N47" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="G48" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" s="35">
+        <v>298</v>
+      </c>
+      <c r="J48" s="65">
+        <v>3.5</v>
+      </c>
       <c r="K48" s="32"/>
       <c r="L48" s="20"/>
-      <c r="M48" s="20"/>
-      <c r="N48" s="20"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A49" s="36"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="35"/>
+      <c r="M48" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N48" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A49" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F49" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" s="35">
+        <v>298</v>
+      </c>
+      <c r="J49" s="65">
+        <v>6.2</v>
+      </c>
       <c r="K49" s="32"/>
       <c r="L49" s="20"/>
-      <c r="M49" s="20"/>
-      <c r="N49" s="20"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="36"/>
-      <c r="C50" s="33"/>
-      <c r="D50" s="33"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="35"/>
+      <c r="M49" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N49" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A50" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>141</v>
+      </c>
+      <c r="C50" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F50" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G50" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="35">
+        <v>298</v>
+      </c>
+      <c r="J50" s="65">
+        <v>7</v>
+      </c>
       <c r="K50" s="32"/>
       <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51" s="36"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="35"/>
+      <c r="M50" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N50" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A51" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
+        <v>142</v>
+      </c>
+      <c r="C51" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F51" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G51" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" s="35">
+        <v>298</v>
+      </c>
+      <c r="J51" s="65">
+        <v>8.1999999999999993</v>
+      </c>
       <c r="K51" s="32"/>
       <c r="L51" s="20"/>
-      <c r="M51" s="20"/>
-      <c r="N51" s="20"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52" s="36"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="35"/>
+      <c r="M51" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N51" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A52" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F52" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G52" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="35">
+        <v>298</v>
+      </c>
+      <c r="J52" s="65">
+        <v>8.5</v>
+      </c>
       <c r="K52" s="32"/>
       <c r="L52" s="20"/>
-      <c r="M52" s="20"/>
-      <c r="N52" s="20"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A53" s="36"/>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
+      <c r="M52" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N52" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A53" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" t="s">
+        <v>139</v>
+      </c>
+      <c r="C53" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E53" s="20"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
+      <c r="F53" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G53" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H53" s="33"/>
-      <c r="I53" s="35"/>
+      <c r="I53" s="35">
+        <v>298</v>
+      </c>
+      <c r="J53" s="32">
+        <f>P53*0.009807*1000000000</f>
+        <v>3470697300</v>
+      </c>
       <c r="K53" s="32"/>
       <c r="L53" s="20"/>
-      <c r="M53" s="20"/>
-      <c r="N53" s="20"/>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A54" s="36"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
+      <c r="M53" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N53" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P53">
+        <v>353.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A54" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E54" s="20"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
+      <c r="F54" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G54" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H54" s="33"/>
-      <c r="I54" s="35"/>
+      <c r="I54" s="35">
+        <v>298</v>
+      </c>
+      <c r="J54" s="32">
+        <f t="shared" ref="J54:J62" si="2">P54*0.009807*1000000000</f>
+        <v>4304292299.999999</v>
+      </c>
       <c r="K54" s="32"/>
       <c r="L54" s="20"/>
-      <c r="M54" s="20"/>
-      <c r="N54" s="20"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A55" s="36"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
+      <c r="M54" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N54" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P54">
+        <v>438.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E55" s="20"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
+      <c r="F55" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G55" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H55" s="33"/>
-      <c r="I55" s="35"/>
+      <c r="I55" s="35">
+        <v>298</v>
+      </c>
+      <c r="J55" s="32">
+        <f t="shared" si="2"/>
+        <v>4587714600</v>
+      </c>
       <c r="K55" s="32"/>
       <c r="L55" s="20"/>
-      <c r="M55" s="20"/>
-      <c r="N55" s="20"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A56" s="36"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
+      <c r="M55" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N55" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P55">
+        <v>467.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A56" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
+        <v>142</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E56" s="20"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
+      <c r="F56" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G56" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H56" s="33"/>
-      <c r="I56" s="35"/>
+      <c r="I56" s="35">
+        <v>298</v>
+      </c>
+      <c r="J56" s="32">
+        <f t="shared" si="2"/>
+        <v>4888789500</v>
+      </c>
       <c r="K56" s="32"/>
       <c r="L56" s="20"/>
-      <c r="M56" s="20"/>
-      <c r="N56" s="20"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" s="36"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
+      <c r="M56" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N56" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P56">
+        <v>498.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A57" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E57" s="20"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
+      <c r="F57" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G57" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H57" s="33"/>
-      <c r="I57" s="35"/>
+      <c r="I57" s="35">
+        <v>298</v>
+      </c>
+      <c r="J57" s="32">
+        <f t="shared" si="2"/>
+        <v>5206536300</v>
+      </c>
       <c r="K57" s="32"/>
       <c r="L57" s="20"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="20"/>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A58" s="36"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
+      <c r="M57" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N57" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P57">
+        <v>530.9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A58" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" t="s">
+        <v>139</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G58" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H58" s="33"/>
-      <c r="I58" s="35"/>
+      <c r="I58" s="35">
+        <v>298</v>
+      </c>
+      <c r="J58" s="32">
+        <f t="shared" si="2"/>
+        <v>3534442800</v>
+      </c>
       <c r="K58" s="32"/>
       <c r="L58" s="20"/>
-      <c r="M58" s="20"/>
-      <c r="N58" s="20"/>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" s="36"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
+      <c r="M58" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N58" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P58">
+        <v>360.4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A59" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F59" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G59" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H59" s="33"/>
-      <c r="I59" s="35"/>
+      <c r="I59" s="35">
+        <v>298</v>
+      </c>
+      <c r="J59" s="32">
+        <f t="shared" si="2"/>
+        <v>4327829100</v>
+      </c>
       <c r="K59" s="32"/>
       <c r="L59" s="20"/>
-      <c r="M59" s="20"/>
-      <c r="N59" s="20"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="36"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
+      <c r="M59" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N59" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P59">
+        <v>441.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A60" s="36" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F60" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G60" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H60" s="33"/>
-      <c r="I60" s="35"/>
+      <c r="I60" s="35">
+        <v>298</v>
+      </c>
+      <c r="J60" s="32">
+        <f t="shared" si="2"/>
+        <v>4866233400</v>
+      </c>
       <c r="K60" s="32"/>
       <c r="L60" s="20"/>
-      <c r="M60" s="20"/>
-      <c r="N60" s="20"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A61" s="36"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
+      <c r="M60" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N60" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P60">
+        <v>496.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A61" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" t="s">
+        <v>142</v>
+      </c>
+      <c r="C61" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D61" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G61" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H61" s="33"/>
-      <c r="I61" s="35"/>
+      <c r="I61" s="35">
+        <v>298</v>
+      </c>
+      <c r="J61" s="32">
+        <f>P61*0.009807*1000000000</f>
+        <v>5098659300</v>
+      </c>
       <c r="K61" s="32"/>
       <c r="L61" s="20"/>
-      <c r="M61" s="20"/>
-      <c r="N61" s="20"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A62" s="36"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
+      <c r="M61" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N61" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P61">
+        <v>519.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A62" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" t="s">
+        <v>143</v>
+      </c>
+      <c r="C62" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D62" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F62" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G62" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H62" s="33"/>
-      <c r="I62" s="35"/>
+      <c r="I62" s="35">
+        <v>298</v>
+      </c>
+      <c r="J62" s="32">
+        <f t="shared" si="2"/>
+        <v>5563511099.999999</v>
+      </c>
       <c r="K62" s="32"/>
       <c r="L62" s="20"/>
-      <c r="M62" s="20"/>
-      <c r="N62" s="20"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A63" s="36"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
+      <c r="M62" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N62" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P62">
+        <v>567.29999999999995</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A63" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D63" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E63" s="20"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
+      <c r="F63" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G63" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H63" s="33"/>
-      <c r="I63" s="35"/>
+      <c r="I63" s="35">
+        <v>293</v>
+      </c>
+      <c r="J63" s="32">
+        <v>9.5749999999999993</v>
+      </c>
       <c r="K63" s="32"/>
-      <c r="L63" s="20"/>
-      <c r="M63" s="20"/>
-      <c r="N63" s="20"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A64" s="36"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
+      <c r="L63" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M63" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N63" s="64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A64" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E64" s="20"/>
-      <c r="F64" s="33"/>
-      <c r="G64" s="33"/>
+      <c r="F64" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G64" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H64" s="33"/>
-      <c r="I64" s="35"/>
+      <c r="I64" s="35">
+        <v>293</v>
+      </c>
+      <c r="J64" s="32">
+        <v>10.324</v>
+      </c>
       <c r="K64" s="32"/>
-      <c r="L64" s="20"/>
-      <c r="M64" s="20"/>
-      <c r="N64" s="20"/>
+      <c r="L64" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M64" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N64" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A65" s="36"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
+      <c r="A65" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B65" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D65" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E65" s="20"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
+      <c r="F65" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G65" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H65" s="33"/>
-      <c r="I65" s="35"/>
+      <c r="I65" s="35">
+        <v>293</v>
+      </c>
+      <c r="J65" s="32">
+        <v>10.32</v>
+      </c>
       <c r="K65" s="32"/>
-      <c r="L65" s="20"/>
-      <c r="M65" s="20"/>
-      <c r="N65" s="20"/>
+      <c r="L65" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M65" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N65" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A66" s="36"/>
-      <c r="C66" s="33"/>
-      <c r="D66" s="33"/>
+      <c r="A66" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B66" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D66" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E66" s="20"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="33"/>
+      <c r="F66" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H66" s="33"/>
-      <c r="I66" s="35"/>
+      <c r="I66" s="35">
+        <v>293</v>
+      </c>
+      <c r="J66" s="32">
+        <v>10.194000000000001</v>
+      </c>
       <c r="K66" s="32"/>
-      <c r="L66" s="20"/>
-      <c r="M66" s="20"/>
-      <c r="N66" s="20"/>
+      <c r="L66" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M66" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N66" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A67" s="36"/>
-      <c r="C67" s="33"/>
-      <c r="D67" s="33"/>
+      <c r="A67" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B67" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67" s="33" t="s">
+        <v>65</v>
+      </c>
       <c r="E67" s="20"/>
-      <c r="F67" s="33"/>
-      <c r="G67" s="33"/>
+      <c r="F67" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G67" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H67" s="33"/>
-      <c r="I67" s="35"/>
+      <c r="I67" s="35">
+        <v>293</v>
+      </c>
+      <c r="J67" s="32">
+        <v>10.055999999999999</v>
+      </c>
       <c r="K67" s="32"/>
-      <c r="L67" s="20"/>
-      <c r="M67" s="20"/>
-      <c r="N67" s="20"/>
+      <c r="L67" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M67" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N67" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A68" s="36"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="33"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="33"/>
-      <c r="G68" s="33"/>
+      <c r="A68" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B68" t="s">
+        <v>139</v>
+      </c>
+      <c r="C68" s="33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D68" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F68" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G68" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H68" s="33"/>
-      <c r="I68" s="35"/>
+      <c r="I68" s="35">
+        <v>293</v>
+      </c>
+      <c r="J68" s="32">
+        <v>9.58</v>
+      </c>
       <c r="K68" s="32"/>
-      <c r="L68" s="20"/>
-      <c r="M68" s="20"/>
-      <c r="N68" s="20"/>
+      <c r="L68" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M68" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N68" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A69" s="36"/>
-      <c r="C69" s="33"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="33"/>
+      <c r="A69" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B69" t="s">
+        <v>140</v>
+      </c>
+      <c r="C69" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D69" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F69" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G69" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H69" s="33"/>
-      <c r="I69" s="35"/>
+      <c r="I69" s="35">
+        <v>293</v>
+      </c>
+      <c r="J69" s="32">
+        <v>9.952</v>
+      </c>
       <c r="K69" s="32"/>
-      <c r="L69" s="20"/>
-      <c r="M69" s="20"/>
-      <c r="N69" s="20"/>
+      <c r="L69" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M69" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N69" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A70" s="36"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="33"/>
+      <c r="A70" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B70" t="s">
+        <v>141</v>
+      </c>
+      <c r="C70" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D70" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F70" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G70" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H70" s="33"/>
-      <c r="I70" s="35"/>
+      <c r="I70" s="35">
+        <v>293</v>
+      </c>
+      <c r="J70" s="32">
+        <v>9.7129999999999992</v>
+      </c>
       <c r="K70" s="32"/>
-      <c r="L70" s="20"/>
-      <c r="M70" s="20"/>
-      <c r="N70" s="20"/>
+      <c r="L70" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M70" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N70" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A71" s="36"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="33"/>
-      <c r="G71" s="33"/>
+      <c r="A71" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B71" t="s">
+        <v>142</v>
+      </c>
+      <c r="C71" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D71" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F71" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G71" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H71" s="33"/>
-      <c r="I71" s="35"/>
+      <c r="I71" s="35">
+        <v>293</v>
+      </c>
+      <c r="J71" s="32">
+        <v>9.6530000000000005</v>
+      </c>
       <c r="K71" s="32"/>
-      <c r="L71" s="20"/>
-      <c r="M71" s="20"/>
-      <c r="N71" s="20"/>
+      <c r="L71" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M71" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N71" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A72" s="36"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="33"/>
-      <c r="G72" s="33"/>
+      <c r="A72" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" t="s">
+        <v>143</v>
+      </c>
+      <c r="C72" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="D72" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F72" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G72" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H72" s="33"/>
-      <c r="I72" s="35"/>
+      <c r="I72" s="35">
+        <v>293</v>
+      </c>
+      <c r="J72" s="32">
+        <v>9.4130000000000003</v>
+      </c>
       <c r="K72" s="32"/>
-      <c r="L72" s="20"/>
-      <c r="M72" s="20"/>
-      <c r="N72" s="20"/>
+      <c r="L72" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="M72" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N72" s="64" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="36"/>
@@ -8094,8 +9503,18 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D357D88A-2775-40B2-B73F-2173296B7938}"/>
     <hyperlink ref="N17" r:id="rId2" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.actamat.2023.118728" xr:uid="{71A6AE26-FBF4-DE45-8238-670CA1EA4EAF}"/>
     <hyperlink ref="N18:N22" r:id="rId3" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.actamat.2023.118728" xr:uid="{C22AB022-BA1F-684B-AA90-8ED5F1D04DDE}"/>
+    <hyperlink ref="N23" r:id="rId4" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{EE6B1F39-147C-3F47-BF0B-B792DF9E1023}"/>
+    <hyperlink ref="N24:N32" r:id="rId5" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{04B0B27D-6C9E-AE4A-8D31-6B0D13275CF6}"/>
+    <hyperlink ref="N33" r:id="rId6" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{F7EDC1E0-8376-9B44-A89A-386CB1B3C2B0}"/>
+    <hyperlink ref="N34:N42" r:id="rId7" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{B84E16FE-52A4-154A-B542-D79D4021B647}"/>
+    <hyperlink ref="N43" r:id="rId8" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{8634E8D2-D623-8F4E-893F-FA2BFD1AE842}"/>
+    <hyperlink ref="N44:N52" r:id="rId9" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{B030A353-134D-8347-AEED-9D62F44FE4FB}"/>
+    <hyperlink ref="N53" r:id="rId10" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{7F2AAADB-EE6F-1843-99CF-884EE570F41A}"/>
+    <hyperlink ref="N54:N62" r:id="rId11" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{8116D0B5-58BA-0A43-AB59-8CA353885F0C}"/>
+    <hyperlink ref="N63" r:id="rId12" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{2C2945FD-F982-4B4A-A02E-4EA25F64ACFF}"/>
+    <hyperlink ref="N64:N72" r:id="rId13" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{5B835531-4C44-5444-9D22-AB43615D1A30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- add 6 multiproperty points from 10.1016/j.ijrmhm.2023.106263 - add 14 multiproperty points from10.1016/j.intermet.2023.107872
</commit_message>
<xml_diff>
--- a/Compilation_HardnessAndDuctility.xlsx
+++ b/Compilation_HardnessAndDuctility.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-contribute-Detor2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81E0C72-6E54-4149-9BDB-40BE5D8A94F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA9B47E-F32F-A943-B18E-81DEF804758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33760" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="166">
   <si>
     <t>Name:</t>
   </si>
@@ -588,6 +588,42 @@
   </si>
   <si>
     <t>density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zr35 Ti30 Nb20 Al10 Ta5 </t>
+  </si>
+  <si>
+    <t>VAM+CR+A+WQ</t>
+  </si>
+  <si>
+    <t>5min at 850*C in argon in quartz tube, B2 nanoprecipitates</t>
+  </si>
+  <si>
+    <t>5min at 1050*C in argon in quartz tube, B2 nanoprecipitates</t>
+  </si>
+  <si>
+    <t>10.1016/j.ijrmhm.2023.106263</t>
+  </si>
+  <si>
+    <t>ultimate tensile strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1016/j.intermet.2023.107872 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zr35 Ti30 Nb20 Al10 V5 </t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2023.107872</t>
+  </si>
+  <si>
+    <t>Zr35 Ti30 Nb20 Al10 Ta5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2 nanoprecipitates </t>
   </si>
 </sst>
 </file>
@@ -1616,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T431"/>
+  <dimension ref="A1:T440"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2483,7 +2519,9 @@
         <v>721000000</v>
       </c>
       <c r="K23" s="32"/>
-      <c r="L23" s="20"/>
+      <c r="L23" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M23" s="20" t="s">
         <v>64</v>
       </c>
@@ -2523,7 +2561,9 @@
         <v>855000000</v>
       </c>
       <c r="K24" s="32"/>
-      <c r="L24" s="20"/>
+      <c r="L24" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M24" s="20" t="s">
         <v>64</v>
       </c>
@@ -2563,7 +2603,9 @@
         <v>932000000</v>
       </c>
       <c r="K25" s="32"/>
-      <c r="L25" s="20"/>
+      <c r="L25" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M25" s="20" t="s">
         <v>64</v>
       </c>
@@ -2603,7 +2645,9 @@
         <v>993000000</v>
       </c>
       <c r="K26" s="32"/>
-      <c r="L26" s="20"/>
+      <c r="L26" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M26" s="20" t="s">
         <v>64</v>
       </c>
@@ -2643,7 +2687,9 @@
         <v>1389000000</v>
       </c>
       <c r="K27" s="32"/>
-      <c r="L27" s="20"/>
+      <c r="L27" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M27" s="20" t="s">
         <v>64</v>
       </c>
@@ -2685,7 +2731,9 @@
         <v>793000000</v>
       </c>
       <c r="K28" s="32"/>
-      <c r="L28" s="20"/>
+      <c r="L28" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M28" s="20" t="s">
         <v>64</v>
       </c>
@@ -2727,7 +2775,9 @@
         <v>945000000</v>
       </c>
       <c r="K29" s="32"/>
-      <c r="L29" s="20"/>
+      <c r="L29" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M29" s="20" t="s">
         <v>64</v>
       </c>
@@ -2769,7 +2819,9 @@
         <v>1021000000</v>
       </c>
       <c r="K30" s="32"/>
-      <c r="L30" s="20"/>
+      <c r="L30" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M30" s="20" t="s">
         <v>64</v>
       </c>
@@ -2811,7 +2863,9 @@
         <v>1181000000</v>
       </c>
       <c r="K31" s="32"/>
-      <c r="L31" s="20"/>
+      <c r="L31" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M31" s="20" t="s">
         <v>64</v>
       </c>
@@ -2853,7 +2907,9 @@
         <v>1502000000</v>
       </c>
       <c r="K32" s="32"/>
-      <c r="L32" s="20"/>
+      <c r="L32" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M32" s="20" t="s">
         <v>64</v>
       </c>
@@ -2893,7 +2949,9 @@
         <v>984000000</v>
       </c>
       <c r="K33" s="32"/>
-      <c r="L33" s="20"/>
+      <c r="L33" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M33" s="20" t="s">
         <v>64</v>
       </c>
@@ -2933,7 +2991,9 @@
         <v>985000000</v>
       </c>
       <c r="K34" s="32"/>
-      <c r="L34" s="20"/>
+      <c r="L34" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M34" s="20" t="s">
         <v>64</v>
       </c>
@@ -2973,7 +3033,9 @@
         <v>1025000000</v>
       </c>
       <c r="K35" s="32"/>
-      <c r="L35" s="20"/>
+      <c r="L35" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M35" s="20" t="s">
         <v>64</v>
       </c>
@@ -3013,7 +3075,9 @@
         <v>1177000000</v>
       </c>
       <c r="K36" s="32"/>
-      <c r="L36" s="20"/>
+      <c r="L36" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M36" s="20" t="s">
         <v>64</v>
       </c>
@@ -3053,7 +3117,9 @@
         <v>1420000000</v>
       </c>
       <c r="K37" s="32"/>
-      <c r="L37" s="20"/>
+      <c r="L37" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M37" s="20" t="s">
         <v>64</v>
       </c>
@@ -3095,7 +3161,9 @@
         <v>1085000000</v>
       </c>
       <c r="K38" s="32"/>
-      <c r="L38" s="20"/>
+      <c r="L38" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M38" s="20" t="s">
         <v>64</v>
       </c>
@@ -3137,7 +3205,9 @@
         <v>980000000</v>
       </c>
       <c r="K39" s="32"/>
-      <c r="L39" s="20"/>
+      <c r="L39" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M39" s="20" t="s">
         <v>64</v>
       </c>
@@ -3179,7 +3249,9 @@
         <v>1081000000</v>
       </c>
       <c r="K40" s="32"/>
-      <c r="L40" s="20"/>
+      <c r="L40" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M40" s="20" t="s">
         <v>64</v>
       </c>
@@ -3221,7 +3293,9 @@
         <v>1221000000</v>
       </c>
       <c r="K41" s="32"/>
-      <c r="L41" s="20"/>
+      <c r="L41" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M41" s="20" t="s">
         <v>64</v>
       </c>
@@ -3263,7 +3337,9 @@
         <v>1548000000</v>
       </c>
       <c r="K42" s="32"/>
-      <c r="L42" s="20"/>
+      <c r="L42" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M42" s="20" t="s">
         <v>64</v>
       </c>
@@ -3301,7 +3377,9 @@
         <v>50</v>
       </c>
       <c r="K43" s="32"/>
-      <c r="L43" s="20"/>
+      <c r="L43" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M43" s="20" t="s">
         <v>64</v>
       </c>
@@ -3336,7 +3414,9 @@
         <v>14.9</v>
       </c>
       <c r="K44" s="32"/>
-      <c r="L44" s="20"/>
+      <c r="L44" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M44" s="20" t="s">
         <v>64</v>
       </c>
@@ -3371,7 +3451,9 @@
         <v>14.2</v>
       </c>
       <c r="K45" s="32"/>
-      <c r="L45" s="20"/>
+      <c r="L45" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M45" s="20" t="s">
         <v>64</v>
       </c>
@@ -3406,7 +3488,9 @@
         <v>12.1</v>
       </c>
       <c r="K46" s="32"/>
-      <c r="L46" s="20"/>
+      <c r="L46" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M46" s="20" t="s">
         <v>64</v>
       </c>
@@ -3441,7 +3525,9 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="K47" s="32"/>
-      <c r="L47" s="20"/>
+      <c r="L47" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M47" s="20" t="s">
         <v>64</v>
       </c>
@@ -3478,7 +3564,9 @@
         <v>3.5</v>
       </c>
       <c r="K48" s="32"/>
-      <c r="L48" s="20"/>
+      <c r="L48" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M48" s="20" t="s">
         <v>64</v>
       </c>
@@ -3515,7 +3603,9 @@
         <v>6.2</v>
       </c>
       <c r="K49" s="32"/>
-      <c r="L49" s="20"/>
+      <c r="L49" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M49" s="20" t="s">
         <v>64</v>
       </c>
@@ -3552,7 +3642,9 @@
         <v>7</v>
       </c>
       <c r="K50" s="32"/>
-      <c r="L50" s="20"/>
+      <c r="L50" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M50" s="20" t="s">
         <v>64</v>
       </c>
@@ -3589,7 +3681,9 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="K51" s="32"/>
-      <c r="L51" s="20"/>
+      <c r="L51" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M51" s="20" t="s">
         <v>64</v>
       </c>
@@ -3626,7 +3720,9 @@
         <v>8.5</v>
       </c>
       <c r="K52" s="32"/>
-      <c r="L52" s="20"/>
+      <c r="L52" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="M52" s="20" t="s">
         <v>64</v>
       </c>
@@ -3663,7 +3759,9 @@
         <v>3470697300</v>
       </c>
       <c r="K53" s="32"/>
-      <c r="L53" s="20"/>
+      <c r="L53" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M53" s="20" t="s">
         <v>64</v>
       </c>
@@ -3703,7 +3801,9 @@
         <v>4304292299.999999</v>
       </c>
       <c r="K54" s="32"/>
-      <c r="L54" s="20"/>
+      <c r="L54" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M54" s="20" t="s">
         <v>64</v>
       </c>
@@ -3743,7 +3843,9 @@
         <v>4587714600</v>
       </c>
       <c r="K55" s="32"/>
-      <c r="L55" s="20"/>
+      <c r="L55" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M55" s="20" t="s">
         <v>64</v>
       </c>
@@ -3783,7 +3885,9 @@
         <v>4888789500</v>
       </c>
       <c r="K56" s="32"/>
-      <c r="L56" s="20"/>
+      <c r="L56" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M56" s="20" t="s">
         <v>64</v>
       </c>
@@ -3823,7 +3927,9 @@
         <v>5206536300</v>
       </c>
       <c r="K57" s="32"/>
-      <c r="L57" s="20"/>
+      <c r="L57" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M57" s="20" t="s">
         <v>64</v>
       </c>
@@ -3865,7 +3971,9 @@
         <v>3534442800</v>
       </c>
       <c r="K58" s="32"/>
-      <c r="L58" s="20"/>
+      <c r="L58" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M58" s="20" t="s">
         <v>64</v>
       </c>
@@ -3907,7 +4015,9 @@
         <v>4327829100</v>
       </c>
       <c r="K59" s="32"/>
-      <c r="L59" s="20"/>
+      <c r="L59" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M59" s="20" t="s">
         <v>64</v>
       </c>
@@ -3949,7 +4059,9 @@
         <v>4866233400</v>
       </c>
       <c r="K60" s="32"/>
-      <c r="L60" s="20"/>
+      <c r="L60" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M60" s="20" t="s">
         <v>64</v>
       </c>
@@ -3991,7 +4103,9 @@
         <v>5098659300</v>
       </c>
       <c r="K61" s="32"/>
-      <c r="L61" s="20"/>
+      <c r="L61" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M61" s="20" t="s">
         <v>64</v>
       </c>
@@ -4033,7 +4147,9 @@
         <v>5563511099.999999</v>
       </c>
       <c r="K62" s="32"/>
-      <c r="L62" s="20"/>
+      <c r="L62" s="20" t="s">
+        <v>42</v>
+      </c>
       <c r="M62" s="20" t="s">
         <v>64</v>
       </c>
@@ -4120,7 +4236,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="36" t="s">
         <v>109</v>
       </c>
@@ -4158,7 +4274,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="36" t="s">
         <v>110</v>
       </c>
@@ -4196,7 +4312,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="36" t="s">
         <v>111</v>
       </c>
@@ -4234,7 +4350,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="36" t="s">
         <v>112</v>
       </c>
@@ -4274,7 +4390,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="36" t="s">
         <v>113</v>
       </c>
@@ -4314,7 +4430,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="36" t="s">
         <v>114</v>
       </c>
@@ -4354,7 +4470,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="36" t="s">
         <v>115</v>
       </c>
@@ -4394,7 +4510,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="36" t="s">
         <v>116</v>
       </c>
@@ -4434,290 +4550,869 @@
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="36"/>
-      <c r="C73" s="33"/>
-      <c r="D73" s="33"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="33"/>
-      <c r="G73" s="33"/>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A73" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" t="s">
+        <v>154</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D73" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E73" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F73" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G73" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H73" s="33"/>
-      <c r="I73" s="35"/>
+      <c r="I73" s="35">
+        <v>298</v>
+      </c>
+      <c r="J73" s="32">
+        <f t="shared" ref="J73:J76" si="3">Q73*1000000</f>
+        <v>997000000</v>
+      </c>
       <c r="K73" s="32"/>
-      <c r="L73" s="20"/>
-      <c r="M73" s="20"/>
-      <c r="N73" s="20"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A74" s="36"/>
-      <c r="C74" s="33"/>
-      <c r="D74" s="33"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="33"/>
-      <c r="G74" s="33"/>
+      <c r="L73" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M73" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N73" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q73">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A74" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B74" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D74" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="F74" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G74" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H74" s="33"/>
-      <c r="I74" s="35"/>
+      <c r="I74" s="35">
+        <v>298</v>
+      </c>
+      <c r="J74" s="32">
+        <f t="shared" si="3"/>
+        <v>841000000</v>
+      </c>
       <c r="K74" s="32"/>
-      <c r="L74" s="20"/>
-      <c r="M74" s="20"/>
-      <c r="N74" s="20"/>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A75" s="36"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
+      <c r="L74" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M74" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N74" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q74">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A75" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D75" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E75" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F75" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G75" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H75" s="33"/>
-      <c r="I75" s="35"/>
+      <c r="I75" s="35">
+        <v>298</v>
+      </c>
+      <c r="J75" s="32">
+        <f t="shared" si="3"/>
+        <v>1043000000</v>
+      </c>
       <c r="K75" s="32"/>
-      <c r="L75" s="20"/>
-      <c r="M75" s="20"/>
-      <c r="N75" s="20"/>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A76" s="36"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
+      <c r="L75" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M75" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N75" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q75">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A76" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D76" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E76" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="F76" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G76" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H76" s="33"/>
-      <c r="I76" s="35"/>
+      <c r="I76" s="35">
+        <v>298</v>
+      </c>
+      <c r="J76" s="32">
+        <f t="shared" si="3"/>
+        <v>857000000</v>
+      </c>
       <c r="K76" s="32"/>
-      <c r="L76" s="20"/>
-      <c r="M76" s="20"/>
-      <c r="N76" s="20"/>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A77" s="36"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="33"/>
+      <c r="L76" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M76" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N76" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q76">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A77" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D77" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E77" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="F77" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G77" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H77" s="33"/>
-      <c r="I77" s="35"/>
+      <c r="I77" s="35">
+        <v>298</v>
+      </c>
+      <c r="J77">
+        <v>20</v>
+      </c>
       <c r="K77" s="32"/>
-      <c r="L77" s="20"/>
-      <c r="M77" s="20"/>
-      <c r="N77" s="20"/>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A78" s="36"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="33"/>
+      <c r="L77" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M77" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N77" s="64" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A78" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B78" t="s">
+        <v>154</v>
+      </c>
+      <c r="C78" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D78" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E78" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="F78" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G78" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H78" s="33"/>
-      <c r="I78" s="35"/>
+      <c r="I78" s="35">
+        <v>298</v>
+      </c>
+      <c r="J78">
+        <v>15</v>
+      </c>
       <c r="K78" s="32"/>
-      <c r="L78" s="20"/>
-      <c r="M78" s="20"/>
-      <c r="N78" s="20"/>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A79" s="36"/>
-      <c r="C79" s="33"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="33"/>
+      <c r="L78" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M78" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N78" s="64" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A79" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" t="s">
+        <v>154</v>
+      </c>
+      <c r="C79" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D79" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E79" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F79" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G79" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H79" s="33"/>
-      <c r="I79" s="35"/>
+      <c r="I79" s="35">
+        <v>298</v>
+      </c>
+      <c r="J79" s="32">
+        <f t="shared" ref="J79" si="4">Q79*1000000</f>
+        <v>850000000</v>
+      </c>
       <c r="K79" s="32"/>
-      <c r="L79" s="20"/>
-      <c r="M79" s="20"/>
-      <c r="N79" s="20"/>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A80" s="36"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
+      <c r="L79" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M79" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N79" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q79">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" t="s">
+        <v>154</v>
+      </c>
+      <c r="C80" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D80" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E80" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F80" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G80" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H80" s="33"/>
-      <c r="I80" s="35"/>
+      <c r="I80" s="35">
+        <v>873</v>
+      </c>
+      <c r="J80" s="32">
+        <f t="shared" ref="J80:J81" si="5">Q80*1000000</f>
+        <v>721000000</v>
+      </c>
       <c r="K80" s="32"/>
-      <c r="L80" s="20"/>
-      <c r="M80" s="20"/>
-      <c r="N80" s="20"/>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A81" s="36"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="33"/>
-      <c r="G81" s="33"/>
+      <c r="L80" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M80" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N80" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q80">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A81" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D81" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E81" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F81" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G81" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H81" s="33"/>
-      <c r="I81" s="35"/>
+      <c r="I81" s="35">
+        <v>1073</v>
+      </c>
+      <c r="J81" s="32">
+        <f t="shared" si="5"/>
+        <v>668000000</v>
+      </c>
       <c r="K81" s="32"/>
-      <c r="L81" s="20"/>
-      <c r="M81" s="20"/>
-      <c r="N81" s="20"/>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A82" s="36"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="33"/>
+      <c r="L81" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M81" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N81" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q81">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A82" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B82" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D82" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E82" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F82" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G82" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H82" s="33"/>
-      <c r="I82" s="35"/>
+      <c r="I82" s="35">
+        <v>298</v>
+      </c>
+      <c r="J82" s="32">
+        <v>25</v>
+      </c>
       <c r="K82" s="32"/>
-      <c r="L82" s="20"/>
-      <c r="M82" s="20"/>
-      <c r="N82" s="20"/>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A83" s="36"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="33"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="33"/>
-      <c r="G83" s="33"/>
+      <c r="L82" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M82" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N82" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A83" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B83" t="s">
+        <v>164</v>
+      </c>
+      <c r="C83" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D83" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E83" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F83" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G83" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H83" s="33"/>
-      <c r="I83" s="35"/>
+      <c r="I83" s="35">
+        <v>873</v>
+      </c>
+      <c r="J83" s="32">
+        <v>23</v>
+      </c>
       <c r="K83" s="32"/>
-      <c r="L83" s="20"/>
-      <c r="M83" s="20"/>
-      <c r="N83" s="20"/>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A84" s="36"/>
-      <c r="C84" s="33"/>
-      <c r="D84" s="33"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="33"/>
-      <c r="G84" s="33"/>
+      <c r="L83" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M83" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N83" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A84" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B84" t="s">
+        <v>164</v>
+      </c>
+      <c r="C84" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D84" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E84" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F84" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G84" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H84" s="33"/>
-      <c r="I84" s="35"/>
+      <c r="I84" s="35">
+        <v>1073</v>
+      </c>
+      <c r="J84" s="32">
+        <v>18</v>
+      </c>
       <c r="K84" s="32"/>
-      <c r="L84" s="20"/>
-      <c r="M84" s="20"/>
-      <c r="N84" s="20"/>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A85" s="36"/>
-      <c r="C85" s="33"/>
-      <c r="D85" s="33"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="33"/>
-      <c r="G85" s="33"/>
+      <c r="L84" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M84" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N84" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A85" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B85" t="s">
+        <v>154</v>
+      </c>
+      <c r="C85" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D85" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E85" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F85" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G85" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H85" s="33"/>
-      <c r="I85" s="35"/>
-      <c r="K85" s="32"/>
-      <c r="L85" s="20"/>
-      <c r="M85" s="20"/>
-      <c r="N85" s="20"/>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A86" s="36"/>
-      <c r="C86" s="33"/>
-      <c r="D86" s="33"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="33"/>
-      <c r="G86" s="33"/>
+      <c r="I85" s="35">
+        <v>298</v>
+      </c>
+      <c r="J85" s="32">
+        <f t="shared" ref="J85:K85" si="6">P85*0.009807*1000000000</f>
+        <v>3049976999.9999995</v>
+      </c>
+      <c r="K85" s="32">
+        <f t="shared" si="6"/>
+        <v>29421000</v>
+      </c>
+      <c r="L85" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M85" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N85" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="P85">
+        <v>311</v>
+      </c>
+      <c r="Q85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A86" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B86" t="s">
+        <v>161</v>
+      </c>
+      <c r="C86" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D86" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E86" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F86" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G86" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H86" s="33"/>
-      <c r="I86" s="35"/>
+      <c r="I86" s="35">
+        <v>298</v>
+      </c>
+      <c r="J86" s="32">
+        <f t="shared" ref="J86:J88" si="7">Q86*1000000</f>
+        <v>848000000</v>
+      </c>
       <c r="K86" s="32"/>
-      <c r="L86" s="20"/>
-      <c r="M86" s="20"/>
-      <c r="N86" s="20"/>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A87" s="36"/>
-      <c r="C87" s="33"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="33"/>
-      <c r="G87" s="33"/>
+      <c r="L86" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M86" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N86" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q86">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A87" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B87" t="s">
+        <v>161</v>
+      </c>
+      <c r="C87" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D87" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E87" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F87" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G87" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H87" s="33"/>
-      <c r="I87" s="35"/>
+      <c r="I87" s="35">
+        <v>873</v>
+      </c>
+      <c r="J87" s="32">
+        <f t="shared" si="7"/>
+        <v>635000000</v>
+      </c>
       <c r="K87" s="32"/>
-      <c r="L87" s="20"/>
-      <c r="M87" s="20"/>
-      <c r="N87" s="20"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A88" s="36"/>
-      <c r="C88" s="33"/>
-      <c r="D88" s="33"/>
-      <c r="E88" s="20"/>
-      <c r="F88" s="33"/>
-      <c r="G88" s="33"/>
+      <c r="L87" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M87" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N87" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q87">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A88" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B88" t="s">
+        <v>161</v>
+      </c>
+      <c r="C88" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D88" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E88" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F88" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="G88" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H88" s="33"/>
-      <c r="I88" s="35"/>
+      <c r="I88" s="35">
+        <v>1073</v>
+      </c>
+      <c r="J88" s="32">
+        <f t="shared" si="7"/>
+        <v>583000000</v>
+      </c>
       <c r="K88" s="32"/>
-      <c r="L88" s="20"/>
-      <c r="M88" s="20"/>
-      <c r="N88" s="20"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A89" s="36"/>
-      <c r="C89" s="33"/>
-      <c r="D89" s="33"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="33"/>
+      <c r="L88" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M88" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N88" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q88">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A89" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B89" t="s">
+        <v>161</v>
+      </c>
+      <c r="C89" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D89" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E89" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F89" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G89" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H89" s="33"/>
-      <c r="I89" s="35"/>
+      <c r="I89" s="35">
+        <v>298</v>
+      </c>
+      <c r="J89">
+        <v>16</v>
+      </c>
       <c r="K89" s="32"/>
-      <c r="L89" s="20"/>
-      <c r="M89" s="20"/>
-      <c r="N89" s="20"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A90" s="36"/>
-      <c r="C90" s="33"/>
-      <c r="D90" s="33"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="33"/>
-      <c r="G90" s="33"/>
+      <c r="L89" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M89" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N89" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A90" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B90" t="s">
+        <v>161</v>
+      </c>
+      <c r="C90" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D90" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E90" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F90" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G90" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H90" s="33"/>
-      <c r="I90" s="35"/>
+      <c r="I90" s="35">
+        <v>873</v>
+      </c>
+      <c r="J90">
+        <v>16</v>
+      </c>
       <c r="K90" s="32"/>
-      <c r="L90" s="20"/>
-      <c r="M90" s="20"/>
-      <c r="N90" s="20"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A91" s="36"/>
-      <c r="C91" s="33"/>
-      <c r="D91" s="33"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="33"/>
-      <c r="G91" s="33"/>
+      <c r="L90" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M90" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N90" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A91" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" t="s">
+        <v>161</v>
+      </c>
+      <c r="C91" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D91" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E91" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F91" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="G91" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H91" s="33"/>
-      <c r="I91" s="35"/>
+      <c r="I91" s="35">
+        <v>1073</v>
+      </c>
+      <c r="J91">
+        <v>14</v>
+      </c>
       <c r="K91" s="32"/>
-      <c r="L91" s="20"/>
-      <c r="M91" s="20"/>
-      <c r="N91" s="20"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A92" s="36"/>
-      <c r="C92" s="33"/>
-      <c r="D92" s="33"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="33"/>
-      <c r="G92" s="33"/>
+      <c r="L91" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M91" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N91" s="64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A92" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B92" t="s">
+        <v>161</v>
+      </c>
+      <c r="C92" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D92" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E92" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="F92" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G92" s="33" t="s">
+        <v>19</v>
+      </c>
       <c r="H92" s="33"/>
-      <c r="I92" s="35"/>
-      <c r="K92" s="32"/>
-      <c r="L92" s="20"/>
-      <c r="M92" s="20"/>
-      <c r="N92" s="20"/>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I92" s="35">
+        <v>298</v>
+      </c>
+      <c r="J92" s="32">
+        <f t="shared" ref="J92:K92" si="8">P92*0.009807*1000000000</f>
+        <v>3079398000</v>
+      </c>
+      <c r="K92" s="32">
+        <f t="shared" si="8"/>
+        <v>49034999.999999993</v>
+      </c>
+      <c r="L92" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M92" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="N92" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="P92">
+        <v>314</v>
+      </c>
+      <c r="Q92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="36"/>
       <c r="C93" s="33"/>
-      <c r="D93" s="33"/>
       <c r="E93" s="20"/>
       <c r="F93" s="33"/>
       <c r="G93" s="33"/>
@@ -4728,7 +5423,7 @@
       <c r="M93" s="20"/>
       <c r="N93" s="20"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="36"/>
       <c r="C94" s="33"/>
       <c r="D94" s="33"/>
@@ -4742,7 +5437,7 @@
       <c r="M94" s="20"/>
       <c r="N94" s="20"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="36"/>
       <c r="C95" s="33"/>
       <c r="D95" s="33"/>
@@ -4756,7 +5451,7 @@
       <c r="M95" s="20"/>
       <c r="N95" s="20"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="36"/>
       <c r="C96" s="33"/>
       <c r="D96" s="33"/>
@@ -5948,7 +6643,6 @@
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181" s="36"/>
-      <c r="B181" s="20"/>
       <c r="C181" s="33"/>
       <c r="D181" s="33"/>
       <c r="E181" s="20"/>
@@ -5963,7 +6657,6 @@
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182" s="36"/>
-      <c r="B182" s="20"/>
       <c r="C182" s="33"/>
       <c r="D182" s="33"/>
       <c r="E182" s="20"/>
@@ -5971,7 +6664,6 @@
       <c r="G182" s="33"/>
       <c r="H182" s="33"/>
       <c r="I182" s="35"/>
-      <c r="J182" s="32"/>
       <c r="K182" s="32"/>
       <c r="L182" s="20"/>
       <c r="M182" s="20"/>
@@ -5979,7 +6671,6 @@
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183" s="36"/>
-      <c r="B183" s="20"/>
       <c r="C183" s="33"/>
       <c r="D183" s="33"/>
       <c r="E183" s="20"/>
@@ -5987,7 +6678,6 @@
       <c r="G183" s="33"/>
       <c r="H183" s="33"/>
       <c r="I183" s="35"/>
-      <c r="J183" s="32"/>
       <c r="K183" s="32"/>
       <c r="L183" s="20"/>
       <c r="M183" s="20"/>
@@ -5995,7 +6685,6 @@
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184" s="36"/>
-      <c r="B184" s="20"/>
       <c r="C184" s="33"/>
       <c r="D184" s="33"/>
       <c r="E184" s="20"/>
@@ -6003,7 +6692,6 @@
       <c r="G184" s="33"/>
       <c r="H184" s="33"/>
       <c r="I184" s="35"/>
-      <c r="J184" s="32"/>
       <c r="K184" s="32"/>
       <c r="L184" s="20"/>
       <c r="M184" s="20"/>
@@ -6011,7 +6699,6 @@
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185" s="36"/>
-      <c r="B185" s="20"/>
       <c r="C185" s="33"/>
       <c r="D185" s="33"/>
       <c r="E185" s="20"/>
@@ -6019,7 +6706,6 @@
       <c r="G185" s="33"/>
       <c r="H185" s="33"/>
       <c r="I185" s="35"/>
-      <c r="J185" s="32"/>
       <c r="K185" s="32"/>
       <c r="L185" s="20"/>
       <c r="M185" s="20"/>
@@ -6027,7 +6713,6 @@
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186" s="36"/>
-      <c r="B186" s="20"/>
       <c r="C186" s="33"/>
       <c r="D186" s="33"/>
       <c r="E186" s="20"/>
@@ -6035,7 +6720,6 @@
       <c r="G186" s="33"/>
       <c r="H186" s="33"/>
       <c r="I186" s="35"/>
-      <c r="J186" s="32"/>
       <c r="K186" s="32"/>
       <c r="L186" s="20"/>
       <c r="M186" s="20"/>
@@ -6043,7 +6727,6 @@
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187" s="36"/>
-      <c r="B187" s="20"/>
       <c r="C187" s="33"/>
       <c r="D187" s="33"/>
       <c r="E187" s="20"/>
@@ -6051,7 +6734,6 @@
       <c r="G187" s="33"/>
       <c r="H187" s="33"/>
       <c r="I187" s="35"/>
-      <c r="J187" s="32"/>
       <c r="K187" s="32"/>
       <c r="L187" s="20"/>
       <c r="M187" s="20"/>
@@ -6059,7 +6741,6 @@
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188" s="36"/>
-      <c r="B188" s="20"/>
       <c r="C188" s="33"/>
       <c r="D188" s="33"/>
       <c r="E188" s="20"/>
@@ -6067,7 +6748,6 @@
       <c r="G188" s="33"/>
       <c r="H188" s="33"/>
       <c r="I188" s="35"/>
-      <c r="J188" s="32"/>
       <c r="K188" s="32"/>
       <c r="L188" s="20"/>
       <c r="M188" s="20"/>
@@ -6075,7 +6755,6 @@
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189" s="36"/>
-      <c r="B189" s="20"/>
       <c r="C189" s="33"/>
       <c r="D189" s="33"/>
       <c r="E189" s="20"/>
@@ -6083,7 +6762,6 @@
       <c r="G189" s="33"/>
       <c r="H189" s="33"/>
       <c r="I189" s="35"/>
-      <c r="J189" s="32"/>
       <c r="K189" s="32"/>
       <c r="L189" s="20"/>
       <c r="M189" s="20"/>
@@ -6099,7 +6777,6 @@
       <c r="G190" s="33"/>
       <c r="H190" s="33"/>
       <c r="I190" s="35"/>
-      <c r="J190" s="32"/>
       <c r="K190" s="32"/>
       <c r="L190" s="20"/>
       <c r="M190" s="20"/>
@@ -7179,8 +7856,9 @@
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A258" s="36"/>
-      <c r="C258" s="34"/>
-      <c r="D258" s="34"/>
+      <c r="B258" s="20"/>
+      <c r="C258" s="33"/>
+      <c r="D258" s="33"/>
       <c r="E258" s="20"/>
       <c r="F258" s="33"/>
       <c r="G258" s="33"/>
@@ -7193,12 +7871,14 @@
       <c r="N258" s="20"/>
     </row>
     <row r="259" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A259" s="1"/>
-      <c r="C259" s="34"/>
-      <c r="D259" s="34"/>
-      <c r="F259" s="34"/>
-      <c r="G259" s="34"/>
-      <c r="H259" s="34"/>
+      <c r="A259" s="36"/>
+      <c r="B259" s="20"/>
+      <c r="C259" s="33"/>
+      <c r="D259" s="33"/>
+      <c r="E259" s="20"/>
+      <c r="F259" s="33"/>
+      <c r="G259" s="33"/>
+      <c r="H259" s="33"/>
       <c r="I259" s="35"/>
       <c r="J259" s="32"/>
       <c r="K259" s="32"/>
@@ -7207,12 +7887,14 @@
       <c r="N259" s="20"/>
     </row>
     <row r="260" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A260" s="1"/>
-      <c r="C260" s="34"/>
-      <c r="D260" s="34"/>
-      <c r="F260" s="34"/>
-      <c r="G260" s="34"/>
-      <c r="H260" s="34"/>
+      <c r="A260" s="36"/>
+      <c r="B260" s="20"/>
+      <c r="C260" s="33"/>
+      <c r="D260" s="33"/>
+      <c r="E260" s="20"/>
+      <c r="F260" s="33"/>
+      <c r="G260" s="33"/>
+      <c r="H260" s="33"/>
       <c r="I260" s="35"/>
       <c r="J260" s="32"/>
       <c r="K260" s="32"/>
@@ -7221,12 +7903,14 @@
       <c r="N260" s="20"/>
     </row>
     <row r="261" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A261" s="1"/>
-      <c r="C261" s="34"/>
-      <c r="D261" s="34"/>
-      <c r="F261" s="34"/>
-      <c r="G261" s="34"/>
-      <c r="H261" s="34"/>
+      <c r="A261" s="36"/>
+      <c r="B261" s="20"/>
+      <c r="C261" s="33"/>
+      <c r="D261" s="33"/>
+      <c r="E261" s="20"/>
+      <c r="F261" s="33"/>
+      <c r="G261" s="33"/>
+      <c r="H261" s="33"/>
       <c r="I261" s="35"/>
       <c r="J261" s="32"/>
       <c r="K261" s="32"/>
@@ -7235,12 +7919,14 @@
       <c r="N261" s="20"/>
     </row>
     <row r="262" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A262" s="1"/>
-      <c r="C262" s="34"/>
-      <c r="D262" s="34"/>
-      <c r="F262" s="34"/>
-      <c r="G262" s="34"/>
-      <c r="H262" s="34"/>
+      <c r="A262" s="36"/>
+      <c r="B262" s="20"/>
+      <c r="C262" s="33"/>
+      <c r="D262" s="33"/>
+      <c r="E262" s="20"/>
+      <c r="F262" s="33"/>
+      <c r="G262" s="33"/>
+      <c r="H262" s="33"/>
       <c r="I262" s="35"/>
       <c r="J262" s="32"/>
       <c r="K262" s="32"/>
@@ -7249,12 +7935,14 @@
       <c r="N262" s="20"/>
     </row>
     <row r="263" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A263" s="1"/>
-      <c r="C263" s="34"/>
-      <c r="D263" s="34"/>
-      <c r="F263" s="34"/>
-      <c r="G263" s="34"/>
-      <c r="H263" s="34"/>
+      <c r="A263" s="36"/>
+      <c r="B263" s="20"/>
+      <c r="C263" s="33"/>
+      <c r="D263" s="33"/>
+      <c r="E263" s="20"/>
+      <c r="F263" s="33"/>
+      <c r="G263" s="33"/>
+      <c r="H263" s="33"/>
       <c r="I263" s="35"/>
       <c r="J263" s="32"/>
       <c r="K263" s="32"/>
@@ -7263,12 +7951,14 @@
       <c r="N263" s="20"/>
     </row>
     <row r="264" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A264" s="1"/>
-      <c r="C264" s="34"/>
-      <c r="D264" s="34"/>
-      <c r="F264" s="34"/>
-      <c r="G264" s="34"/>
-      <c r="H264" s="34"/>
+      <c r="A264" s="36"/>
+      <c r="B264" s="20"/>
+      <c r="C264" s="33"/>
+      <c r="D264" s="33"/>
+      <c r="E264" s="20"/>
+      <c r="F264" s="33"/>
+      <c r="G264" s="33"/>
+      <c r="H264" s="33"/>
       <c r="I264" s="35"/>
       <c r="J264" s="32"/>
       <c r="K264" s="32"/>
@@ -7277,12 +7967,14 @@
       <c r="N264" s="20"/>
     </row>
     <row r="265" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A265" s="1"/>
-      <c r="C265" s="34"/>
-      <c r="D265" s="34"/>
-      <c r="F265" s="34"/>
-      <c r="G265" s="34"/>
-      <c r="H265" s="34"/>
+      <c r="A265" s="36"/>
+      <c r="B265" s="20"/>
+      <c r="C265" s="33"/>
+      <c r="D265" s="33"/>
+      <c r="E265" s="20"/>
+      <c r="F265" s="33"/>
+      <c r="G265" s="33"/>
+      <c r="H265" s="33"/>
       <c r="I265" s="35"/>
       <c r="J265" s="32"/>
       <c r="K265" s="32"/>
@@ -7291,12 +7983,14 @@
       <c r="N265" s="20"/>
     </row>
     <row r="266" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A266" s="1"/>
-      <c r="C266" s="34"/>
-      <c r="D266" s="34"/>
-      <c r="F266" s="34"/>
-      <c r="G266" s="34"/>
-      <c r="H266" s="34"/>
+      <c r="A266" s="36"/>
+      <c r="B266" s="20"/>
+      <c r="C266" s="33"/>
+      <c r="D266" s="33"/>
+      <c r="E266" s="20"/>
+      <c r="F266" s="33"/>
+      <c r="G266" s="33"/>
+      <c r="H266" s="33"/>
       <c r="I266" s="35"/>
       <c r="J266" s="32"/>
       <c r="K266" s="32"/>
@@ -7305,12 +7999,13 @@
       <c r="N266" s="20"/>
     </row>
     <row r="267" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A267" s="1"/>
+      <c r="A267" s="36"/>
       <c r="C267" s="34"/>
       <c r="D267" s="34"/>
-      <c r="F267" s="34"/>
-      <c r="G267" s="34"/>
-      <c r="H267" s="34"/>
+      <c r="E267" s="20"/>
+      <c r="F267" s="33"/>
+      <c r="G267" s="33"/>
+      <c r="H267" s="33"/>
       <c r="I267" s="35"/>
       <c r="J267" s="32"/>
       <c r="K267" s="32"/>
@@ -7851,6 +8546,7 @@
       <c r="N305" s="20"/>
     </row>
     <row r="306" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A306" s="1"/>
       <c r="C306" s="34"/>
       <c r="D306" s="34"/>
       <c r="F306" s="34"/>
@@ -7864,6 +8560,7 @@
       <c r="N306" s="20"/>
     </row>
     <row r="307" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A307" s="1"/>
       <c r="C307" s="34"/>
       <c r="D307" s="34"/>
       <c r="F307" s="34"/>
@@ -7877,6 +8574,7 @@
       <c r="N307" s="20"/>
     </row>
     <row r="308" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A308" s="1"/>
       <c r="C308" s="34"/>
       <c r="D308" s="34"/>
       <c r="F308" s="34"/>
@@ -7890,6 +8588,7 @@
       <c r="N308" s="20"/>
     </row>
     <row r="309" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A309" s="1"/>
       <c r="C309" s="34"/>
       <c r="D309" s="34"/>
       <c r="F309" s="34"/>
@@ -7903,6 +8602,7 @@
       <c r="N309" s="20"/>
     </row>
     <row r="310" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A310" s="1"/>
       <c r="C310" s="34"/>
       <c r="D310" s="34"/>
       <c r="F310" s="34"/>
@@ -7916,6 +8616,7 @@
       <c r="N310" s="20"/>
     </row>
     <row r="311" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A311" s="1"/>
       <c r="C311" s="34"/>
       <c r="D311" s="34"/>
       <c r="F311" s="34"/>
@@ -7929,6 +8630,7 @@
       <c r="N311" s="20"/>
     </row>
     <row r="312" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A312" s="1"/>
       <c r="C312" s="34"/>
       <c r="D312" s="34"/>
       <c r="F312" s="34"/>
@@ -7942,6 +8644,7 @@
       <c r="N312" s="20"/>
     </row>
     <row r="313" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A313" s="1"/>
       <c r="C313" s="34"/>
       <c r="D313" s="34"/>
       <c r="F313" s="34"/>
@@ -7955,6 +8658,7 @@
       <c r="N313" s="20"/>
     </row>
     <row r="314" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A314" s="1"/>
       <c r="C314" s="34"/>
       <c r="D314" s="34"/>
       <c r="F314" s="34"/>
@@ -9463,6 +10167,8 @@
       <c r="N429" s="20"/>
     </row>
     <row r="430" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C430" s="34"/>
+      <c r="D430" s="34"/>
       <c r="F430" s="34"/>
       <c r="G430" s="34"/>
       <c r="H430" s="34"/>
@@ -9474,7 +10180,122 @@
       <c r="N430" s="20"/>
     </row>
     <row r="431" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C431" s="34"/>
+      <c r="D431" s="34"/>
+      <c r="F431" s="34"/>
+      <c r="G431" s="34"/>
+      <c r="H431" s="34"/>
+      <c r="I431" s="35"/>
+      <c r="J431" s="32"/>
+      <c r="K431" s="32"/>
+      <c r="L431" s="20"/>
+      <c r="M431" s="20"/>
       <c r="N431" s="20"/>
+    </row>
+    <row r="432" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C432" s="34"/>
+      <c r="D432" s="34"/>
+      <c r="F432" s="34"/>
+      <c r="G432" s="34"/>
+      <c r="H432" s="34"/>
+      <c r="I432" s="35"/>
+      <c r="J432" s="32"/>
+      <c r="K432" s="32"/>
+      <c r="L432" s="20"/>
+      <c r="M432" s="20"/>
+      <c r="N432" s="20"/>
+    </row>
+    <row r="433" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C433" s="34"/>
+      <c r="D433" s="34"/>
+      <c r="F433" s="34"/>
+      <c r="G433" s="34"/>
+      <c r="H433" s="34"/>
+      <c r="I433" s="35"/>
+      <c r="J433" s="32"/>
+      <c r="K433" s="32"/>
+      <c r="L433" s="20"/>
+      <c r="M433" s="20"/>
+      <c r="N433" s="20"/>
+    </row>
+    <row r="434" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C434" s="34"/>
+      <c r="D434" s="34"/>
+      <c r="F434" s="34"/>
+      <c r="G434" s="34"/>
+      <c r="H434" s="34"/>
+      <c r="I434" s="35"/>
+      <c r="J434" s="32"/>
+      <c r="K434" s="32"/>
+      <c r="L434" s="20"/>
+      <c r="M434" s="20"/>
+      <c r="N434" s="20"/>
+    </row>
+    <row r="435" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C435" s="34"/>
+      <c r="D435" s="34"/>
+      <c r="F435" s="34"/>
+      <c r="G435" s="34"/>
+      <c r="H435" s="34"/>
+      <c r="I435" s="35"/>
+      <c r="J435" s="32"/>
+      <c r="K435" s="32"/>
+      <c r="L435" s="20"/>
+      <c r="M435" s="20"/>
+      <c r="N435" s="20"/>
+    </row>
+    <row r="436" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C436" s="34"/>
+      <c r="D436" s="34"/>
+      <c r="F436" s="34"/>
+      <c r="G436" s="34"/>
+      <c r="H436" s="34"/>
+      <c r="I436" s="35"/>
+      <c r="J436" s="32"/>
+      <c r="K436" s="32"/>
+      <c r="L436" s="20"/>
+      <c r="M436" s="20"/>
+      <c r="N436" s="20"/>
+    </row>
+    <row r="437" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C437" s="34"/>
+      <c r="D437" s="34"/>
+      <c r="F437" s="34"/>
+      <c r="G437" s="34"/>
+      <c r="H437" s="34"/>
+      <c r="I437" s="35"/>
+      <c r="J437" s="32"/>
+      <c r="K437" s="32"/>
+      <c r="L437" s="20"/>
+      <c r="M437" s="20"/>
+      <c r="N437" s="20"/>
+    </row>
+    <row r="438" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C438" s="34"/>
+      <c r="D438" s="34"/>
+      <c r="F438" s="34"/>
+      <c r="G438" s="34"/>
+      <c r="H438" s="34"/>
+      <c r="I438" s="35"/>
+      <c r="J438" s="32"/>
+      <c r="K438" s="32"/>
+      <c r="L438" s="20"/>
+      <c r="M438" s="20"/>
+      <c r="N438" s="20"/>
+    </row>
+    <row r="439" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F439" s="34"/>
+      <c r="G439" s="34"/>
+      <c r="H439" s="34"/>
+      <c r="I439" s="35"/>
+      <c r="J439" s="32"/>
+      <c r="K439" s="32"/>
+      <c r="L439" s="20"/>
+      <c r="M439" s="20"/>
+      <c r="N439" s="20"/>
+    </row>
+    <row r="440" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="N440" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -9513,8 +10334,14 @@
     <hyperlink ref="N54:N62" r:id="rId11" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{8116D0B5-58BA-0A43-AB59-8CA353885F0C}"/>
     <hyperlink ref="N63" r:id="rId12" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{2C2945FD-F982-4B4A-A02E-4EA25F64ACFF}"/>
     <hyperlink ref="N64:N72" r:id="rId13" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.jallcom.2022.166593" xr:uid="{5B835531-4C44-5444-9D22-AB43615D1A30}"/>
+    <hyperlink ref="N73" r:id="rId14" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{FDE28797-5232-E549-9AA2-0463FA382B94}"/>
+    <hyperlink ref="N74" r:id="rId15" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{56725AFC-1BEC-4241-A33F-0DA7AC464098}"/>
+    <hyperlink ref="N75" r:id="rId16" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{AA80762B-5075-ED4C-9B1F-824B10A6D221}"/>
+    <hyperlink ref="N76" r:id="rId17" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{5A5D038C-E9E4-0F4A-B2EE-896B04C40BFD}"/>
+    <hyperlink ref="N77" r:id="rId18" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{A3B80E8B-6CA1-DA47-B749-E049C7CD09D5}"/>
+    <hyperlink ref="N78" r:id="rId19" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{7E2D3582-8C6E-2246-83D8-A1A37C81467D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(Sufyan 2022) - added 34 unary/binary D parameters
</commit_message>
<xml_diff>
--- a/Compilation_HardnessAndDuctility.xlsx
+++ b/Compilation_HardnessAndDuctility.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-contribute-Detor2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA9B47E-F32F-A943-B18E-81DEF804758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90433704-1401-E549-A03C-B87861144AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33760" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="205">
   <si>
     <t>Name:</t>
   </si>
@@ -624,6 +624,123 @@
   </si>
   <si>
     <t xml:space="preserve">B2 nanoprecipitates </t>
+  </si>
+  <si>
+    <t>10.1016/j.jallcom.2022.168597</t>
+  </si>
+  <si>
+    <t>TiW</t>
+  </si>
+  <si>
+    <t>TiMo</t>
+  </si>
+  <si>
+    <t>TiTa</t>
+  </si>
+  <si>
+    <t>TiNb</t>
+  </si>
+  <si>
+    <t>TiV</t>
+  </si>
+  <si>
+    <t>TiTi</t>
+  </si>
+  <si>
+    <t>ZrMo</t>
+  </si>
+  <si>
+    <t>ZrTa</t>
+  </si>
+  <si>
+    <t>ZrNb</t>
+  </si>
+  <si>
+    <t>ZrZr</t>
+  </si>
+  <si>
+    <t>HfW</t>
+  </si>
+  <si>
+    <t>HfMo</t>
+  </si>
+  <si>
+    <t>HfTa</t>
+  </si>
+  <si>
+    <t>HfNb</t>
+  </si>
+  <si>
+    <t>HfHf</t>
+  </si>
+  <si>
+    <t>VW</t>
+  </si>
+  <si>
+    <t>VMo</t>
+  </si>
+  <si>
+    <t>VTa</t>
+  </si>
+  <si>
+    <t>VNb</t>
+  </si>
+  <si>
+    <t>VV</t>
+  </si>
+  <si>
+    <t>NbRe</t>
+  </si>
+  <si>
+    <t>NbW</t>
+  </si>
+  <si>
+    <t>NbMo</t>
+  </si>
+  <si>
+    <t>NbTa</t>
+  </si>
+  <si>
+    <t>NbNb</t>
+  </si>
+  <si>
+    <t>TaW</t>
+  </si>
+  <si>
+    <t>TaMo</t>
+  </si>
+  <si>
+    <t>TaTa</t>
+  </si>
+  <si>
+    <t>MoRe</t>
+  </si>
+  <si>
+    <t>MoW</t>
+  </si>
+  <si>
+    <t>MoMo</t>
+  </si>
+  <si>
+    <t>WRe</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>ReRe</t>
+  </si>
+  <si>
+    <t>d parameter</t>
+  </si>
+  <si>
+    <t>DFT</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>SQS 128-atom supercell</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1291,6 +1408,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1342,35 +1488,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1654,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K97" sqref="K97"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,19 +1809,19 @@
       <c r="B2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1713,17 +1831,17 @@
       <c r="B3" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="41"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
       <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1741,43 +1859,43 @@
       <c r="B5" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="55" t="s">
+      <c r="M5" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="55" t="s">
+      <c r="N5" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="56" t="s">
+      <c r="O5" s="40" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1788,19 +1906,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="57"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="41"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1845,7 +1963,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="58"/>
+      <c r="O7" s="42"/>
       <c r="P7" s="31" t="s">
         <v>126</v>
       </c>
@@ -1858,35 +1976,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="52" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="53"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="59" t="s">
+      <c r="P8" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="61"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="45"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2288,7 +2406,7 @@
       <c r="M17" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N17" s="64" t="s">
+      <c r="N17" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2328,7 +2446,7 @@
       <c r="M18" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N18" s="64" t="s">
+      <c r="N18" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2368,7 +2486,7 @@
       <c r="M19" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N19" s="64" t="s">
+      <c r="N19" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2406,7 +2524,7 @@
       <c r="M20" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N20" s="64" t="s">
+      <c r="N20" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2446,7 +2564,7 @@
       <c r="M21" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N21" s="64" t="s">
+      <c r="N21" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2486,7 +2604,7 @@
       <c r="M22" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N22" s="64" t="s">
+      <c r="N22" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2525,7 +2643,7 @@
       <c r="M23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="64" t="s">
+      <c r="N23" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q23">
@@ -2567,7 +2685,7 @@
       <c r="M24" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N24" s="64" t="s">
+      <c r="N24" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q24">
@@ -2609,7 +2727,7 @@
       <c r="M25" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="64" t="s">
+      <c r="N25" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q25">
@@ -2651,7 +2769,7 @@
       <c r="M26" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N26" s="64" t="s">
+      <c r="N26" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q26">
@@ -2693,7 +2811,7 @@
       <c r="M27" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N27" s="64" t="s">
+      <c r="N27" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q27">
@@ -2737,7 +2855,7 @@
       <c r="M28" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N28" s="64" t="s">
+      <c r="N28" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q28">
@@ -2781,7 +2899,7 @@
       <c r="M29" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N29" s="64" t="s">
+      <c r="N29" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q29">
@@ -2825,7 +2943,7 @@
       <c r="M30" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N30" s="64" t="s">
+      <c r="N30" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q30">
@@ -2869,7 +2987,7 @@
       <c r="M31" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="64" t="s">
+      <c r="N31" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q31">
@@ -2913,7 +3031,7 @@
       <c r="M32" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="64" t="s">
+      <c r="N32" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q32">
@@ -2955,7 +3073,7 @@
       <c r="M33" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N33" s="64" t="s">
+      <c r="N33" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q33">
@@ -2997,7 +3115,7 @@
       <c r="M34" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N34" s="64" t="s">
+      <c r="N34" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q34">
@@ -3039,7 +3157,7 @@
       <c r="M35" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N35" s="64" t="s">
+      <c r="N35" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q35">
@@ -3081,7 +3199,7 @@
       <c r="M36" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N36" s="64" t="s">
+      <c r="N36" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q36">
@@ -3123,7 +3241,7 @@
       <c r="M37" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N37" s="64" t="s">
+      <c r="N37" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q37">
@@ -3167,7 +3285,7 @@
       <c r="M38" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N38" s="64" t="s">
+      <c r="N38" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q38">
@@ -3211,7 +3329,7 @@
       <c r="M39" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N39" s="64" t="s">
+      <c r="N39" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q39">
@@ -3255,7 +3373,7 @@
       <c r="M40" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N40" s="64" t="s">
+      <c r="N40" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q40">
@@ -3299,7 +3417,7 @@
       <c r="M41" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N41" s="64" t="s">
+      <c r="N41" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q41">
@@ -3343,7 +3461,7 @@
       <c r="M42" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N42" s="64" t="s">
+      <c r="N42" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q42">
@@ -3373,7 +3491,7 @@
       <c r="I43" s="35">
         <v>298</v>
       </c>
-      <c r="J43" s="65">
+      <c r="J43" s="39">
         <v>50</v>
       </c>
       <c r="K43" s="32"/>
@@ -3383,7 +3501,7 @@
       <c r="M43" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N43" s="64" t="s">
+      <c r="N43" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3410,7 +3528,7 @@
       <c r="I44" s="35">
         <v>298</v>
       </c>
-      <c r="J44" s="65">
+      <c r="J44" s="39">
         <v>14.9</v>
       </c>
       <c r="K44" s="32"/>
@@ -3420,7 +3538,7 @@
       <c r="M44" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N44" s="64" t="s">
+      <c r="N44" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3447,7 +3565,7 @@
       <c r="I45" s="35">
         <v>298</v>
       </c>
-      <c r="J45" s="65">
+      <c r="J45" s="39">
         <v>14.2</v>
       </c>
       <c r="K45" s="32"/>
@@ -3457,7 +3575,7 @@
       <c r="M45" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N45" s="64" t="s">
+      <c r="N45" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3484,7 +3602,7 @@
       <c r="I46" s="35">
         <v>298</v>
       </c>
-      <c r="J46" s="65">
+      <c r="J46" s="39">
         <v>12.1</v>
       </c>
       <c r="K46" s="32"/>
@@ -3494,7 +3612,7 @@
       <c r="M46" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N46" s="64" t="s">
+      <c r="N46" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3521,7 +3639,7 @@
       <c r="I47" s="35">
         <v>298</v>
       </c>
-      <c r="J47" s="65">
+      <c r="J47" s="39">
         <v>9.1999999999999993</v>
       </c>
       <c r="K47" s="32"/>
@@ -3531,7 +3649,7 @@
       <c r="M47" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N47" s="64" t="s">
+      <c r="N47" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3560,7 +3678,7 @@
       <c r="I48" s="35">
         <v>298</v>
       </c>
-      <c r="J48" s="65">
+      <c r="J48" s="39">
         <v>3.5</v>
       </c>
       <c r="K48" s="32"/>
@@ -3570,7 +3688,7 @@
       <c r="M48" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N48" s="64" t="s">
+      <c r="N48" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3599,7 +3717,7 @@
       <c r="I49" s="35">
         <v>298</v>
       </c>
-      <c r="J49" s="65">
+      <c r="J49" s="39">
         <v>6.2</v>
       </c>
       <c r="K49" s="32"/>
@@ -3609,7 +3727,7 @@
       <c r="M49" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N49" s="64" t="s">
+      <c r="N49" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3638,7 +3756,7 @@
       <c r="I50" s="35">
         <v>298</v>
       </c>
-      <c r="J50" s="65">
+      <c r="J50" s="39">
         <v>7</v>
       </c>
       <c r="K50" s="32"/>
@@ -3648,7 +3766,7 @@
       <c r="M50" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N50" s="64" t="s">
+      <c r="N50" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3677,7 +3795,7 @@
       <c r="I51" s="35">
         <v>298</v>
       </c>
-      <c r="J51" s="65">
+      <c r="J51" s="39">
         <v>8.1999999999999993</v>
       </c>
       <c r="K51" s="32"/>
@@ -3687,7 +3805,7 @@
       <c r="M51" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N51" s="64" t="s">
+      <c r="N51" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3716,7 +3834,7 @@
       <c r="I52" s="35">
         <v>298</v>
       </c>
-      <c r="J52" s="65">
+      <c r="J52" s="39">
         <v>8.5</v>
       </c>
       <c r="K52" s="32"/>
@@ -3726,7 +3844,7 @@
       <c r="M52" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N52" s="64" t="s">
+      <c r="N52" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3765,7 +3883,7 @@
       <c r="M53" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N53" s="64" t="s">
+      <c r="N53" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P53">
@@ -3807,7 +3925,7 @@
       <c r="M54" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N54" s="64" t="s">
+      <c r="N54" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P54">
@@ -3849,7 +3967,7 @@
       <c r="M55" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N55" s="64" t="s">
+      <c r="N55" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P55">
@@ -3891,7 +4009,7 @@
       <c r="M56" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N56" s="64" t="s">
+      <c r="N56" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P56">
@@ -3933,7 +4051,7 @@
       <c r="M57" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N57" s="64" t="s">
+      <c r="N57" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P57">
@@ -3977,7 +4095,7 @@
       <c r="M58" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N58" s="64" t="s">
+      <c r="N58" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P58">
@@ -4021,7 +4139,7 @@
       <c r="M59" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N59" s="64" t="s">
+      <c r="N59" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P59">
@@ -4065,7 +4183,7 @@
       <c r="M60" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N60" s="64" t="s">
+      <c r="N60" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P60">
@@ -4109,7 +4227,7 @@
       <c r="M61" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N61" s="64" t="s">
+      <c r="N61" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P61">
@@ -4153,7 +4271,7 @@
       <c r="M62" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N62" s="64" t="s">
+      <c r="N62" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P62">
@@ -4194,7 +4312,7 @@
       <c r="M63" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N63" s="64" t="s">
+      <c r="N63" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4232,7 +4350,7 @@
       <c r="M64" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N64" s="64" t="s">
+      <c r="N64" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4270,7 +4388,7 @@
       <c r="M65" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N65" s="64" t="s">
+      <c r="N65" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4308,7 +4426,7 @@
       <c r="M66" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N66" s="64" t="s">
+      <c r="N66" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4346,7 +4464,7 @@
       <c r="M67" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N67" s="64" t="s">
+      <c r="N67" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4386,7 +4504,7 @@
       <c r="M68" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N68" s="64" t="s">
+      <c r="N68" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4426,7 +4544,7 @@
       <c r="M69" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N69" s="64" t="s">
+      <c r="N69" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4466,7 +4584,7 @@
       <c r="M70" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N70" s="64" t="s">
+      <c r="N70" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4506,7 +4624,7 @@
       <c r="M71" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N71" s="64" t="s">
+      <c r="N71" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4546,7 +4664,7 @@
       <c r="M72" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N72" s="64" t="s">
+      <c r="N72" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4587,7 +4705,7 @@
       <c r="M73" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N73" s="64" t="s">
+      <c r="N73" s="38" t="s">
         <v>158</v>
       </c>
       <c r="Q73">
@@ -4631,7 +4749,7 @@
       <c r="M74" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N74" s="64" t="s">
+      <c r="N74" s="38" t="s">
         <v>158</v>
       </c>
       <c r="Q74">
@@ -4675,7 +4793,7 @@
       <c r="M75" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N75" s="64" t="s">
+      <c r="N75" s="38" t="s">
         <v>158</v>
       </c>
       <c r="Q75">
@@ -4719,7 +4837,7 @@
       <c r="M76" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N76" s="64" t="s">
+      <c r="N76" s="38" t="s">
         <v>158</v>
       </c>
       <c r="Q76">
@@ -4762,7 +4880,7 @@
       <c r="M77" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N77" s="64" t="s">
+      <c r="N77" s="38" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4802,7 +4920,7 @@
       <c r="M78" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N78" s="64" t="s">
+      <c r="N78" s="38" t="s">
         <v>158</v>
       </c>
     </row>
@@ -4843,7 +4961,7 @@
       <c r="M79" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N79" s="64" t="s">
+      <c r="N79" s="38" t="s">
         <v>160</v>
       </c>
       <c r="Q79">
@@ -4887,7 +5005,7 @@
       <c r="M80" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N80" s="64" t="s">
+      <c r="N80" s="38" t="s">
         <v>160</v>
       </c>
       <c r="Q80">
@@ -4931,7 +5049,7 @@
       <c r="M81" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N81" s="64" t="s">
+      <c r="N81" s="38" t="s">
         <v>163</v>
       </c>
       <c r="Q81">
@@ -4974,7 +5092,7 @@
       <c r="M82" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N82" s="64" t="s">
+      <c r="N82" s="38" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5014,7 +5132,7 @@
       <c r="M83" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N83" s="64" t="s">
+      <c r="N83" s="38" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5054,7 +5172,7 @@
       <c r="M84" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N84" s="64" t="s">
+      <c r="N84" s="38" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5098,7 +5216,7 @@
       <c r="M85" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N85" s="64" t="s">
+      <c r="N85" s="38" t="s">
         <v>163</v>
       </c>
       <c r="P85">
@@ -5145,7 +5263,7 @@
       <c r="M86" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N86" s="64" t="s">
+      <c r="N86" s="38" t="s">
         <v>163</v>
       </c>
       <c r="Q86">
@@ -5189,7 +5307,7 @@
       <c r="M87" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N87" s="64" t="s">
+      <c r="N87" s="38" t="s">
         <v>163</v>
       </c>
       <c r="Q87">
@@ -5233,7 +5351,7 @@
       <c r="M88" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N88" s="64" t="s">
+      <c r="N88" s="38" t="s">
         <v>163</v>
       </c>
       <c r="Q88">
@@ -5276,7 +5394,7 @@
       <c r="M89" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N89" s="64" t="s">
+      <c r="N89" s="38" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5316,7 +5434,7 @@
       <c r="M90" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N90" s="64" t="s">
+      <c r="N90" s="38" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5356,7 +5474,7 @@
       <c r="M91" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N91" s="64" t="s">
+      <c r="N91" s="38" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5400,7 +5518,7 @@
       <c r="M92" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="N92" s="64" t="s">
+      <c r="N92" s="38" t="s">
         <v>163</v>
       </c>
       <c r="P92">
@@ -5411,479 +5529,1227 @@
       </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A93" s="36"/>
-      <c r="C93" s="33"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="33"/>
-      <c r="G93" s="33"/>
+      <c r="A93" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B93" t="s">
+        <v>167</v>
+      </c>
+      <c r="C93" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E93" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F93" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G93" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H93" s="33"/>
-      <c r="I93" s="35"/>
+      <c r="I93" s="35">
+        <v>0</v>
+      </c>
+      <c r="J93" s="39">
+        <v>2.6247240618101544</v>
+      </c>
       <c r="K93" s="32"/>
       <c r="L93" s="20"/>
-      <c r="M93" s="20"/>
-      <c r="N93" s="20"/>
+      <c r="M93" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N93" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A94" s="36"/>
-      <c r="C94" s="33"/>
+      <c r="A94" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="B94" t="s">
+        <v>168</v>
+      </c>
+      <c r="C94" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D94" s="33"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="33"/>
-      <c r="G94" s="33"/>
+      <c r="E94" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F94" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G94" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H94" s="33"/>
-      <c r="I94" s="35"/>
+      <c r="I94" s="35">
+        <v>0</v>
+      </c>
+      <c r="J94" s="39">
+        <v>2.5918128654970762</v>
+      </c>
       <c r="K94" s="32"/>
       <c r="L94" s="20"/>
-      <c r="M94" s="20"/>
-      <c r="N94" s="20"/>
+      <c r="M94" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N94" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A95" s="36"/>
-      <c r="C95" s="33"/>
+      <c r="A95" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B95" t="s">
+        <v>169</v>
+      </c>
+      <c r="C95" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D95" s="33"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="33"/>
-      <c r="G95" s="33"/>
+      <c r="E95" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F95" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G95" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H95" s="33"/>
-      <c r="I95" s="35"/>
+      <c r="I95" s="35">
+        <v>0</v>
+      </c>
+      <c r="J95" s="39">
+        <v>4.1580041580041582</v>
+      </c>
       <c r="K95" s="32"/>
       <c r="L95" s="20"/>
-      <c r="M95" s="20"/>
-      <c r="N95" s="20"/>
+      <c r="M95" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N95" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A96" s="36"/>
-      <c r="C96" s="33"/>
+      <c r="A96" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96" t="s">
+        <v>170</v>
+      </c>
+      <c r="C96" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D96" s="33"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="33"/>
-      <c r="G96" s="33"/>
+      <c r="E96" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F96" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G96" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H96" s="33"/>
-      <c r="I96" s="35"/>
+      <c r="I96" s="35">
+        <v>0</v>
+      </c>
+      <c r="J96" s="39">
+        <v>3.8817427385892116</v>
+      </c>
       <c r="K96" s="32"/>
       <c r="L96" s="20"/>
-      <c r="M96" s="20"/>
-      <c r="N96" s="20"/>
+      <c r="M96" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N96" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A97" s="36"/>
-      <c r="C97" s="33"/>
+      <c r="A97" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B97" t="s">
+        <v>171</v>
+      </c>
+      <c r="C97" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D97" s="33"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="33"/>
-      <c r="G97" s="33"/>
+      <c r="E97" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F97" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G97" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H97" s="33"/>
-      <c r="I97" s="35"/>
+      <c r="I97" s="35">
+        <v>0</v>
+      </c>
+      <c r="J97" s="39">
+        <v>3.7015209125475286</v>
+      </c>
       <c r="K97" s="32"/>
       <c r="L97" s="20"/>
-      <c r="M97" s="20"/>
-      <c r="N97" s="20"/>
+      <c r="M97" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N97" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A98" s="36"/>
-      <c r="C98" s="33"/>
+      <c r="A98" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B98" t="s">
+        <v>172</v>
+      </c>
+      <c r="C98" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D98" s="33"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="33"/>
-      <c r="G98" s="33"/>
+      <c r="E98" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F98" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G98" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H98" s="33"/>
-      <c r="I98" s="35"/>
+      <c r="I98" s="35">
+        <v>0</v>
+      </c>
+      <c r="J98" s="39">
+        <v>4.2095032397408207</v>
+      </c>
       <c r="K98" s="32"/>
       <c r="L98" s="20"/>
-      <c r="M98" s="20"/>
-      <c r="N98" s="20"/>
+      <c r="M98" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N98" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A99" s="36"/>
-      <c r="C99" s="33"/>
+      <c r="A99" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B99" t="s">
+        <v>173</v>
+      </c>
+      <c r="C99" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D99" s="33"/>
-      <c r="E99" s="20"/>
-      <c r="F99" s="33"/>
-      <c r="G99" s="33"/>
+      <c r="E99" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F99" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G99" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H99" s="33"/>
-      <c r="I99" s="35"/>
+      <c r="I99" s="35">
+        <v>0</v>
+      </c>
+      <c r="J99" s="39">
+        <v>2.5917767988252569</v>
+      </c>
       <c r="K99" s="32"/>
       <c r="L99" s="20"/>
-      <c r="M99" s="20"/>
-      <c r="N99" s="20"/>
+      <c r="M99" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N99" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A100" s="36"/>
-      <c r="C100" s="33"/>
+      <c r="A100" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B100" t="s">
+        <v>174</v>
+      </c>
+      <c r="C100" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D100" s="33"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="33"/>
-      <c r="G100" s="33"/>
+      <c r="E100" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F100" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G100" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H100" s="33"/>
-      <c r="I100" s="35"/>
+      <c r="I100" s="35">
+        <v>0</v>
+      </c>
+      <c r="J100" s="39">
+        <v>3.7907488986784141</v>
+      </c>
       <c r="K100" s="32"/>
       <c r="L100" s="20"/>
-      <c r="M100" s="20"/>
-      <c r="N100" s="20"/>
+      <c r="M100" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N100" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A101" s="36"/>
-      <c r="C101" s="33"/>
+      <c r="A101" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B101" t="s">
+        <v>175</v>
+      </c>
+      <c r="C101" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D101" s="33"/>
-      <c r="E101" s="20"/>
-      <c r="F101" s="33"/>
-      <c r="G101" s="33"/>
+      <c r="E101" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F101" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G101" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H101" s="33"/>
-      <c r="I101" s="35"/>
+      <c r="I101" s="35">
+        <v>0</v>
+      </c>
+      <c r="J101" s="39">
+        <v>3.7098214285714284</v>
+      </c>
       <c r="K101" s="32"/>
       <c r="L101" s="20"/>
-      <c r="M101" s="20"/>
-      <c r="N101" s="20"/>
+      <c r="M101" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N101" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A102" s="36"/>
-      <c r="C102" s="33"/>
+      <c r="A102" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B102" t="s">
+        <v>176</v>
+      </c>
+      <c r="C102" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D102" s="33"/>
-      <c r="E102" s="20"/>
-      <c r="F102" s="33"/>
-      <c r="G102" s="33"/>
+      <c r="E102" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F102" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G102" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H102" s="33"/>
-      <c r="I102" s="35"/>
+      <c r="I102" s="35">
+        <v>0</v>
+      </c>
+      <c r="J102" s="39">
+        <v>3.4704595185995624</v>
+      </c>
       <c r="K102" s="32"/>
       <c r="L102" s="20"/>
-      <c r="M102" s="20"/>
-      <c r="N102" s="20"/>
+      <c r="M102" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N102" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A103" s="36"/>
-      <c r="C103" s="33"/>
+      <c r="A103" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B103" t="s">
+        <v>177</v>
+      </c>
+      <c r="C103" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D103" s="33"/>
-      <c r="E103" s="20"/>
-      <c r="F103" s="33"/>
-      <c r="G103" s="33"/>
+      <c r="E103" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F103" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G103" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H103" s="33"/>
-      <c r="I103" s="35"/>
+      <c r="I103" s="35">
+        <v>0</v>
+      </c>
+      <c r="J103" s="39">
+        <v>2.5187878787878786</v>
+      </c>
       <c r="K103" s="32"/>
       <c r="L103" s="20"/>
-      <c r="M103" s="20"/>
-      <c r="N103" s="20"/>
+      <c r="M103" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N103" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A104" s="36"/>
-      <c r="C104" s="33"/>
+      <c r="A104" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B104" t="s">
+        <v>178</v>
+      </c>
+      <c r="C104" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D104" s="33"/>
-      <c r="E104" s="20"/>
-      <c r="F104" s="33"/>
-      <c r="G104" s="33"/>
+      <c r="E104" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F104" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G104" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H104" s="33"/>
-      <c r="I104" s="35"/>
+      <c r="I104" s="35">
+        <v>0</v>
+      </c>
+      <c r="J104" s="39">
+        <v>2.4722222222222223</v>
+      </c>
       <c r="K104" s="32"/>
       <c r="L104" s="20"/>
-      <c r="M104" s="20"/>
-      <c r="N104" s="20"/>
+      <c r="M104" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N104" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A105" s="36"/>
-      <c r="C105" s="33"/>
+      <c r="A105" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B105" t="s">
+        <v>179</v>
+      </c>
+      <c r="C105" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D105" s="33"/>
-      <c r="E105" s="20"/>
-      <c r="F105" s="33"/>
-      <c r="G105" s="33"/>
+      <c r="E105" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F105" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G105" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H105" s="33"/>
-      <c r="I105" s="35"/>
+      <c r="I105" s="35">
+        <v>0</v>
+      </c>
+      <c r="J105" s="39">
+        <v>3.8272357723577235</v>
+      </c>
       <c r="K105" s="32"/>
       <c r="L105" s="20"/>
-      <c r="M105" s="20"/>
-      <c r="N105" s="20"/>
+      <c r="M105" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N105" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A106" s="36"/>
-      <c r="C106" s="33"/>
+      <c r="A106" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B106" t="s">
+        <v>180</v>
+      </c>
+      <c r="C106" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D106" s="33"/>
-      <c r="E106" s="20"/>
-      <c r="F106" s="33"/>
-      <c r="G106" s="33"/>
+      <c r="E106" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F106" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G106" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H106" s="33"/>
-      <c r="I106" s="35"/>
+      <c r="I106" s="35">
+        <v>0</v>
+      </c>
+      <c r="J106" s="39">
+        <v>3.6733067729083664</v>
+      </c>
       <c r="K106" s="32"/>
       <c r="L106" s="20"/>
-      <c r="M106" s="20"/>
-      <c r="N106" s="20"/>
+      <c r="M106" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N106" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A107" s="36"/>
-      <c r="C107" s="33"/>
+      <c r="A107" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B107" t="s">
+        <v>181</v>
+      </c>
+      <c r="C107" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D107" s="33"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="33"/>
-      <c r="G107" s="33"/>
+      <c r="E107" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F107" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G107" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H107" s="33"/>
-      <c r="I107" s="35"/>
+      <c r="I107" s="35">
+        <v>0</v>
+      </c>
+      <c r="J107" s="39">
+        <v>2.8314238952536823</v>
+      </c>
       <c r="K107" s="32"/>
       <c r="L107" s="20"/>
-      <c r="M107" s="20"/>
-      <c r="N107" s="20"/>
+      <c r="M107" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N107" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A108" s="36"/>
-      <c r="C108" s="33"/>
+      <c r="A108" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B108" t="s">
+        <v>182</v>
+      </c>
+      <c r="C108" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D108" s="33"/>
-      <c r="E108" s="20"/>
-      <c r="F108" s="33"/>
-      <c r="G108" s="33"/>
+      <c r="E108" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F108" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G108" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H108" s="33"/>
-      <c r="I108" s="35"/>
+      <c r="I108" s="35">
+        <v>0</v>
+      </c>
+      <c r="J108" s="39">
+        <v>2.3805970149253732</v>
+      </c>
       <c r="K108" s="32"/>
       <c r="L108" s="20"/>
-      <c r="M108" s="20"/>
-      <c r="N108" s="20"/>
+      <c r="M108" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N108" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A109" s="36"/>
-      <c r="C109" s="33"/>
+      <c r="A109" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B109" t="s">
+        <v>183</v>
+      </c>
+      <c r="C109" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D109" s="33"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="33"/>
-      <c r="G109" s="33"/>
+      <c r="E109" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F109" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G109" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H109" s="33"/>
-      <c r="I109" s="35"/>
+      <c r="I109" s="35">
+        <v>0</v>
+      </c>
+      <c r="J109" s="39">
+        <v>2.0970266040688577</v>
+      </c>
       <c r="K109" s="32"/>
       <c r="L109" s="20"/>
-      <c r="M109" s="20"/>
-      <c r="N109" s="20"/>
+      <c r="M109" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N109" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A110" s="36"/>
-      <c r="C110" s="33"/>
+      <c r="A110" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B110" t="s">
+        <v>184</v>
+      </c>
+      <c r="C110" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D110" s="33"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="33"/>
-      <c r="G110" s="33"/>
+      <c r="E110" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F110" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G110" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H110" s="33"/>
-      <c r="I110" s="35"/>
+      <c r="I110" s="35">
+        <v>0</v>
+      </c>
+      <c r="J110" s="39">
+        <v>3.5944363103953147</v>
+      </c>
       <c r="K110" s="32"/>
       <c r="L110" s="20"/>
-      <c r="M110" s="20"/>
-      <c r="N110" s="20"/>
+      <c r="M110" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N110" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A111" s="36"/>
-      <c r="C111" s="33"/>
+      <c r="A111" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B111" t="s">
+        <v>185</v>
+      </c>
+      <c r="C111" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D111" s="33"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="33"/>
-      <c r="G111" s="33"/>
+      <c r="E111" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F111" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G111" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H111" s="33"/>
-      <c r="I111" s="35"/>
+      <c r="I111" s="35">
+        <v>0</v>
+      </c>
+      <c r="J111" s="39">
+        <v>3.6253918495297808</v>
+      </c>
       <c r="K111" s="32"/>
       <c r="L111" s="20"/>
-      <c r="M111" s="20"/>
-      <c r="N111" s="20"/>
+      <c r="M111" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N111" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A112" s="36"/>
-      <c r="C112" s="33"/>
+      <c r="A112" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B112" t="s">
+        <v>186</v>
+      </c>
+      <c r="C112" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D112" s="33"/>
-      <c r="E112" s="20"/>
-      <c r="F112" s="33"/>
-      <c r="G112" s="33"/>
+      <c r="E112" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F112" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G112" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H112" s="33"/>
-      <c r="I112" s="35"/>
+      <c r="I112" s="35">
+        <v>0</v>
+      </c>
+      <c r="J112" s="39">
+        <v>3.470160116448326</v>
+      </c>
       <c r="K112" s="32"/>
       <c r="L112" s="20"/>
-      <c r="M112" s="20"/>
-      <c r="N112" s="20"/>
+      <c r="M112" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N112" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A113" s="36"/>
-      <c r="C113" s="33"/>
+      <c r="A113" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B113" t="s">
+        <v>187</v>
+      </c>
+      <c r="C113" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D113" s="33"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="33"/>
-      <c r="G113" s="33"/>
+      <c r="E113" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F113" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G113" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H113" s="33"/>
-      <c r="I113" s="35"/>
+      <c r="I113" s="35">
+        <v>0</v>
+      </c>
+      <c r="J113" s="39">
+        <v>2.1929133858267718</v>
+      </c>
       <c r="K113" s="32"/>
       <c r="L113" s="20"/>
-      <c r="M113" s="20"/>
-      <c r="N113" s="20"/>
+      <c r="M113" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N113" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A114" s="36"/>
-      <c r="C114" s="33"/>
+      <c r="A114" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B114" t="s">
+        <v>188</v>
+      </c>
+      <c r="C114" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D114" s="33"/>
-      <c r="E114" s="20"/>
-      <c r="F114" s="33"/>
-      <c r="G114" s="33"/>
+      <c r="E114" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F114" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G114" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H114" s="33"/>
-      <c r="I114" s="35"/>
+      <c r="I114" s="35">
+        <v>0</v>
+      </c>
+      <c r="J114" s="39">
+        <v>2.2335375191424194</v>
+      </c>
       <c r="K114" s="32"/>
       <c r="L114" s="20"/>
-      <c r="M114" s="20"/>
-      <c r="N114" s="20"/>
+      <c r="M114" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N114" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A115" s="36"/>
-      <c r="C115" s="33"/>
+      <c r="A115" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="B115" t="s">
+        <v>189</v>
+      </c>
+      <c r="C115" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D115" s="33"/>
-      <c r="E115" s="20"/>
-      <c r="F115" s="33"/>
-      <c r="G115" s="33"/>
+      <c r="E115" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F115" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G115" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H115" s="33"/>
-      <c r="I115" s="35"/>
+      <c r="I115" s="35">
+        <v>0</v>
+      </c>
+      <c r="J115" s="39">
+        <v>1.9614779874213837</v>
+      </c>
       <c r="K115" s="32"/>
       <c r="L115" s="20"/>
-      <c r="M115" s="20"/>
-      <c r="N115" s="20"/>
+      <c r="M115" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N115" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A116" s="36"/>
-      <c r="C116" s="33"/>
+      <c r="A116" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B116" t="s">
+        <v>190</v>
+      </c>
+      <c r="C116" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D116" s="33"/>
-      <c r="E116" s="20"/>
-      <c r="F116" s="33"/>
-      <c r="G116" s="33"/>
+      <c r="E116" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F116" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G116" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H116" s="33"/>
-      <c r="I116" s="35"/>
+      <c r="I116" s="35">
+        <v>0</v>
+      </c>
+      <c r="J116" s="39">
+        <v>3.2804154302670625</v>
+      </c>
       <c r="K116" s="32"/>
       <c r="L116" s="20"/>
-      <c r="M116" s="20"/>
-      <c r="N116" s="20"/>
+      <c r="M116" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N116" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A117" s="36"/>
-      <c r="C117" s="33"/>
+      <c r="A117" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B117" t="s">
+        <v>191</v>
+      </c>
+      <c r="C117" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D117" s="33"/>
-      <c r="E117" s="20"/>
-      <c r="F117" s="33"/>
-      <c r="G117" s="33"/>
+      <c r="E117" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F117" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G117" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H117" s="33"/>
-      <c r="I117" s="35"/>
+      <c r="I117" s="35">
+        <v>0</v>
+      </c>
+      <c r="J117" s="39">
+        <v>3.0761194029850745</v>
+      </c>
       <c r="K117" s="32"/>
       <c r="L117" s="20"/>
-      <c r="M117" s="20"/>
-      <c r="N117" s="20"/>
+      <c r="M117" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N117" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A118" s="36"/>
-      <c r="C118" s="33"/>
+      <c r="A118" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B118" t="s">
+        <v>192</v>
+      </c>
+      <c r="C118" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D118" s="33"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="33"/>
-      <c r="G118" s="33"/>
+      <c r="E118" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F118" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G118" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H118" s="33"/>
-      <c r="I118" s="35"/>
+      <c r="I118" s="35">
+        <v>0</v>
+      </c>
+      <c r="J118" s="39">
+        <v>2.1139430284857572</v>
+      </c>
       <c r="K118" s="32"/>
       <c r="L118" s="20"/>
-      <c r="M118" s="20"/>
-      <c r="N118" s="20"/>
+      <c r="M118" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N118" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A119" s="36"/>
-      <c r="C119" s="33"/>
+      <c r="A119" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B119" t="s">
+        <v>193</v>
+      </c>
+      <c r="C119" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D119" s="33"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="33"/>
-      <c r="G119" s="33"/>
+      <c r="E119" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F119" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G119" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H119" s="33"/>
-      <c r="I119" s="35"/>
+      <c r="I119" s="35">
+        <v>0</v>
+      </c>
+      <c r="J119" s="39">
+        <v>1.8919687277896233</v>
+      </c>
       <c r="K119" s="32"/>
       <c r="L119" s="20"/>
-      <c r="M119" s="20"/>
-      <c r="N119" s="20"/>
+      <c r="M119" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N119" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A120" s="36"/>
-      <c r="C120" s="33"/>
+      <c r="A120" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B120" t="s">
+        <v>194</v>
+      </c>
+      <c r="C120" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D120" s="33"/>
-      <c r="E120" s="20"/>
-      <c r="F120" s="33"/>
-      <c r="G120" s="33"/>
+      <c r="E120" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F120" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G120" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H120" s="33"/>
-      <c r="I120" s="35"/>
+      <c r="I120" s="35">
+        <v>0</v>
+      </c>
+      <c r="J120" s="39">
+        <v>3.2267759562841531</v>
+      </c>
       <c r="K120" s="32"/>
       <c r="L120" s="20"/>
-      <c r="M120" s="20"/>
-      <c r="N120" s="20"/>
+      <c r="M120" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N120" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A121" s="36"/>
-      <c r="C121" s="33"/>
+      <c r="A121" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B121" t="s">
+        <v>195</v>
+      </c>
+      <c r="C121" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D121" s="33"/>
-      <c r="E121" s="20"/>
-      <c r="F121" s="33"/>
-      <c r="G121" s="33"/>
+      <c r="E121" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F121" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G121" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H121" s="33"/>
-      <c r="I121" s="35"/>
+      <c r="I121" s="35">
+        <v>0</v>
+      </c>
+      <c r="J121" s="39">
+        <v>3.1507311586051743</v>
+      </c>
       <c r="K121" s="32"/>
       <c r="L121" s="20"/>
-      <c r="M121" s="20"/>
-      <c r="N121" s="20"/>
+      <c r="M121" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N121" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A122" s="36"/>
-      <c r="C122" s="33"/>
+      <c r="A122" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B122" t="s">
+        <v>196</v>
+      </c>
+      <c r="C122" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D122" s="33"/>
-      <c r="E122" s="20"/>
-      <c r="F122" s="33"/>
-      <c r="G122" s="33"/>
+      <c r="E122" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F122" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G122" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H122" s="33"/>
-      <c r="I122" s="35"/>
+      <c r="I122" s="35">
+        <v>0</v>
+      </c>
+      <c r="J122" s="39">
+        <v>1.8114217727543129</v>
+      </c>
       <c r="K122" s="32"/>
       <c r="L122" s="20"/>
-      <c r="M122" s="20"/>
-      <c r="N122" s="20"/>
+      <c r="M122" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N122" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A123" s="36"/>
-      <c r="C123" s="33"/>
+      <c r="A123" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B123" t="s">
+        <v>197</v>
+      </c>
+      <c r="C123" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D123" s="33"/>
-      <c r="E123" s="20"/>
-      <c r="F123" s="33"/>
-      <c r="G123" s="33"/>
+      <c r="E123" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F123" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G123" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H123" s="33"/>
-      <c r="I123" s="35"/>
+      <c r="I123" s="35">
+        <v>0</v>
+      </c>
+      <c r="J123" s="39">
+        <v>1.9623693379790941</v>
+      </c>
       <c r="K123" s="32"/>
       <c r="L123" s="20"/>
-      <c r="M123" s="20"/>
-      <c r="N123" s="20"/>
+      <c r="M123" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N123" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A124" s="36"/>
-      <c r="C124" s="33"/>
+      <c r="A124" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B124" t="s">
+        <v>198</v>
+      </c>
+      <c r="C124" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D124" s="33"/>
-      <c r="E124" s="20"/>
-      <c r="F124" s="33"/>
-      <c r="G124" s="33"/>
+      <c r="E124" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F124" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G124" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H124" s="33"/>
-      <c r="I124" s="35"/>
+      <c r="I124" s="35">
+        <v>0</v>
+      </c>
+      <c r="J124" s="39">
+        <v>2.7615101289134438</v>
+      </c>
       <c r="K124" s="32"/>
       <c r="L124" s="20"/>
-      <c r="M124" s="20"/>
-      <c r="N124" s="20"/>
+      <c r="M124" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N124" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A125" s="36"/>
-      <c r="C125" s="33"/>
+      <c r="A125" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B125" t="s">
+        <v>199</v>
+      </c>
+      <c r="C125" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D125" s="33"/>
-      <c r="E125" s="20"/>
-      <c r="F125" s="33"/>
-      <c r="G125" s="33"/>
+      <c r="E125" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F125" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G125" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H125" s="33"/>
-      <c r="I125" s="35"/>
+      <c r="I125" s="35">
+        <v>0</v>
+      </c>
+      <c r="J125" s="39">
+        <v>1.8426395939086295</v>
+      </c>
       <c r="K125" s="32"/>
       <c r="L125" s="20"/>
-      <c r="M125" s="20"/>
-      <c r="N125" s="20"/>
+      <c r="M125" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N125" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A126" s="36"/>
-      <c r="C126" s="33"/>
+      <c r="A126" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="B126" t="s">
+        <v>200</v>
+      </c>
+      <c r="C126" s="33" t="s">
+        <v>125</v>
+      </c>
       <c r="D126" s="33"/>
-      <c r="E126" s="20"/>
-      <c r="F126" s="33"/>
-      <c r="G126" s="33"/>
+      <c r="E126" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="F126" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="G126" s="33" t="s">
+        <v>202</v>
+      </c>
       <c r="H126" s="33"/>
-      <c r="I126" s="35"/>
+      <c r="I126" s="35">
+        <v>0</v>
+      </c>
+      <c r="J126" s="39">
+        <v>1.6432673899170389</v>
+      </c>
       <c r="K126" s="32"/>
       <c r="L126" s="20"/>
-      <c r="M126" s="20"/>
-      <c r="N126" s="20"/>
+      <c r="M126" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="N126" s="66" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="36"/>
@@ -10299,11 +11165,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10318,6 +11179,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -10340,8 +11206,42 @@
     <hyperlink ref="N76" r:id="rId17" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{5A5D038C-E9E4-0F4A-B2EE-896B04C40BFD}"/>
     <hyperlink ref="N77" r:id="rId18" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{A3B80E8B-6CA1-DA47-B749-E049C7CD09D5}"/>
     <hyperlink ref="N78" r:id="rId19" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.ijrmhm.2023.106263" xr:uid="{7E2D3582-8C6E-2246-83D8-A1A37C81467D}"/>
+    <hyperlink ref="N93" r:id="rId20" xr:uid="{B0298C7A-6A21-4243-9DB4-11BB40EA222A}"/>
+    <hyperlink ref="N94" r:id="rId21" xr:uid="{2A77BA37-E283-4B47-99C9-F28EFF73CF46}"/>
+    <hyperlink ref="N95" r:id="rId22" xr:uid="{47F45EBC-100E-364C-8770-B66015BF7B09}"/>
+    <hyperlink ref="N97" r:id="rId23" xr:uid="{34C84F3D-F2E3-B54B-B1F1-66AE6741C716}"/>
+    <hyperlink ref="N99" r:id="rId24" xr:uid="{DE17BD53-2935-4A49-AAAF-B11F73867280}"/>
+    <hyperlink ref="N101" r:id="rId25" xr:uid="{91C40E48-4CBE-3B4E-882D-E61420FA22BC}"/>
+    <hyperlink ref="N103" r:id="rId26" xr:uid="{E949B766-382F-E441-8150-DADF82D2007E}"/>
+    <hyperlink ref="N105" r:id="rId27" xr:uid="{681C3249-ED6B-9A4C-B34C-778C6F808C2D}"/>
+    <hyperlink ref="N96" r:id="rId28" xr:uid="{5C1E9011-1512-AA4C-A336-54D7CC283D68}"/>
+    <hyperlink ref="N98" r:id="rId29" xr:uid="{67EC7832-E4F0-3140-B205-20BAB64F2538}"/>
+    <hyperlink ref="N100" r:id="rId30" xr:uid="{87593BC8-6B1E-EF42-8C4A-ED0217EBD95F}"/>
+    <hyperlink ref="N102" r:id="rId31" xr:uid="{4B4448FA-83B8-2D46-A0D9-12C307113543}"/>
+    <hyperlink ref="N104" r:id="rId32" xr:uid="{31DE62CC-2BE4-704E-A9E7-C123607B2DB8}"/>
+    <hyperlink ref="N107" r:id="rId33" xr:uid="{79D36C3D-050F-E84F-AFCC-661DB857F9A4}"/>
+    <hyperlink ref="N113" r:id="rId34" xr:uid="{412207A4-6B8C-444F-8A2A-D40732D257A0}"/>
+    <hyperlink ref="N119" r:id="rId35" xr:uid="{F1899A39-A788-0040-BA12-E7E14C910E1D}"/>
+    <hyperlink ref="N125" r:id="rId36" xr:uid="{3562C7E2-D9D4-404D-AE12-21504350D897}"/>
+    <hyperlink ref="N109" r:id="rId37" xr:uid="{FB798449-F50E-DC48-8F11-4ADF2C703585}"/>
+    <hyperlink ref="N115" r:id="rId38" xr:uid="{2DC60ED0-54DE-FA4E-AB0A-2D3D8BA15568}"/>
+    <hyperlink ref="N121" r:id="rId39" xr:uid="{35AF99A1-AA21-DE42-86C8-127CC6039F92}"/>
+    <hyperlink ref="N111" r:id="rId40" xr:uid="{D69FDE8E-99EA-0D4C-B11F-560BBE91A22D}"/>
+    <hyperlink ref="N117" r:id="rId41" xr:uid="{FCB2EC10-518E-334E-99E6-C81E6BDB07EE}"/>
+    <hyperlink ref="N123" r:id="rId42" xr:uid="{6CADFEF1-9F0B-E741-B38D-27150EF23729}"/>
+    <hyperlink ref="N106" r:id="rId43" xr:uid="{E7E33F8D-CA37-414D-9E8D-6E16B11C4777}"/>
+    <hyperlink ref="N112" r:id="rId44" xr:uid="{28A19FAD-D0A2-1B44-805F-C1F1A293E33D}"/>
+    <hyperlink ref="N118" r:id="rId45" xr:uid="{7D2F25A3-5E29-2240-83F5-F580E86AA107}"/>
+    <hyperlink ref="N124" r:id="rId46" xr:uid="{C543CF01-40EB-AD41-8B91-51D1498FFD46}"/>
+    <hyperlink ref="N108" r:id="rId47" xr:uid="{2F55D37F-8784-C440-9F43-5BBA32D95FA0}"/>
+    <hyperlink ref="N114" r:id="rId48" xr:uid="{F591F9C9-70E3-D948-9DD1-ED059A8081AC}"/>
+    <hyperlink ref="N120" r:id="rId49" xr:uid="{7D45ECB1-0C50-614C-8DB0-FA6ECC7399F3}"/>
+    <hyperlink ref="N126" r:id="rId50" xr:uid="{630D85C8-DB77-B04B-BFDF-F6F75CCFCA9C}"/>
+    <hyperlink ref="N110" r:id="rId51" xr:uid="{D87C79AE-0D9F-3E41-9D90-E4E9AF819697}"/>
+    <hyperlink ref="N116" r:id="rId52" xr:uid="{73F7361F-6459-A540-BE00-9C3E4B68A757}"/>
+    <hyperlink ref="N122" r:id="rId53" xr:uid="{672AAEF2-9073-5C46-A048-DD0B84211BF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- adjusted density from `g/cm^3` to `kg/m^3` for compliance with ULTERA schema
</commit_message>
<xml_diff>
--- a/Compilation_HardnessAndDuctility.xlsx
+++ b/Compilation_HardnessAndDuctility.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-contribute-Detor2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA9B47E-F32F-A943-B18E-81DEF804758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A925131-B2A3-B64C-A5B1-8FAFA12C6C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33760" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -578,9 +578,6 @@
     <t>compressive ductility</t>
   </si>
   <si>
-    <t>g/cm^3</t>
-  </si>
-  <si>
     <t>compressive yield strength</t>
   </si>
   <si>
@@ -624,6 +621,9 @@
   </si>
   <si>
     <t xml:space="preserve">B2 nanoprecipitates </t>
+  </si>
+  <si>
+    <t>kg/m3</t>
   </si>
 </sst>
 </file>
@@ -1291,6 +1291,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1342,35 +1371,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1654,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K97" sqref="K97"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M98" sqref="M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,19 +1691,19 @@
       <c r="B2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1713,17 +1713,17 @@
       <c r="B3" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="41"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
       <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1741,43 +1741,43 @@
       <c r="B5" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="62" t="s">
+      <c r="H5" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="55" t="s">
+      <c r="K5" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="55" t="s">
+      <c r="M5" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="55" t="s">
+      <c r="N5" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="56" t="s">
+      <c r="O5" s="40" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1788,19 +1788,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="57"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="41"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1845,7 +1845,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="58"/>
+      <c r="O7" s="42"/>
       <c r="P7" s="31" t="s">
         <v>126</v>
       </c>
@@ -1858,35 +1858,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="52" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="53"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="59" t="s">
+      <c r="P8" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="60"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="61"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="45"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2288,7 +2288,7 @@
       <c r="M17" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N17" s="64" t="s">
+      <c r="N17" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2328,7 +2328,7 @@
       <c r="M18" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N18" s="64" t="s">
+      <c r="N18" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2368,7 +2368,7 @@
       <c r="M19" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N19" s="64" t="s">
+      <c r="N19" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2406,7 +2406,7 @@
       <c r="M20" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N20" s="64" t="s">
+      <c r="N20" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2446,7 +2446,7 @@
       <c r="M21" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N21" s="64" t="s">
+      <c r="N21" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2486,7 +2486,7 @@
       <c r="M22" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="N22" s="64" t="s">
+      <c r="N22" s="38" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2505,7 +2505,7 @@
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G23" s="33" t="s">
         <v>19</v>
@@ -2525,7 +2525,7 @@
       <c r="M23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N23" s="64" t="s">
+      <c r="N23" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q23">
@@ -2547,7 +2547,7 @@
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G24" s="33" t="s">
         <v>19</v>
@@ -2567,7 +2567,7 @@
       <c r="M24" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N24" s="64" t="s">
+      <c r="N24" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q24">
@@ -2589,7 +2589,7 @@
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G25" s="33" t="s">
         <v>19</v>
@@ -2609,7 +2609,7 @@
       <c r="M25" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N25" s="64" t="s">
+      <c r="N25" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q25">
@@ -2631,7 +2631,7 @@
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G26" s="33" t="s">
         <v>19</v>
@@ -2651,7 +2651,7 @@
       <c r="M26" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N26" s="64" t="s">
+      <c r="N26" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q26">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G27" s="33" t="s">
         <v>19</v>
@@ -2693,7 +2693,7 @@
       <c r="M27" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N27" s="64" t="s">
+      <c r="N27" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q27">
@@ -2717,7 +2717,7 @@
         <v>146</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G28" s="33" t="s">
         <v>19</v>
@@ -2737,7 +2737,7 @@
       <c r="M28" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N28" s="64" t="s">
+      <c r="N28" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q28">
@@ -2761,7 +2761,7 @@
         <v>146</v>
       </c>
       <c r="F29" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G29" s="33" t="s">
         <v>19</v>
@@ -2781,7 +2781,7 @@
       <c r="M29" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N29" s="64" t="s">
+      <c r="N29" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q29">
@@ -2805,7 +2805,7 @@
         <v>146</v>
       </c>
       <c r="F30" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G30" s="33" t="s">
         <v>19</v>
@@ -2825,7 +2825,7 @@
       <c r="M30" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N30" s="64" t="s">
+      <c r="N30" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q30">
@@ -2849,7 +2849,7 @@
         <v>146</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G31" s="33" t="s">
         <v>19</v>
@@ -2869,7 +2869,7 @@
       <c r="M31" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="64" t="s">
+      <c r="N31" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q31">
@@ -2893,7 +2893,7 @@
         <v>146</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G32" s="33" t="s">
         <v>19</v>
@@ -2913,7 +2913,7 @@
       <c r="M32" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="64" t="s">
+      <c r="N32" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q32">
@@ -2935,7 +2935,7 @@
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G33" s="33" t="s">
         <v>19</v>
@@ -2955,7 +2955,7 @@
       <c r="M33" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N33" s="64" t="s">
+      <c r="N33" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q33">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G34" s="33" t="s">
         <v>19</v>
@@ -2997,7 +2997,7 @@
       <c r="M34" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N34" s="64" t="s">
+      <c r="N34" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q34">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G35" s="33" t="s">
         <v>19</v>
@@ -3039,7 +3039,7 @@
       <c r="M35" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N35" s="64" t="s">
+      <c r="N35" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q35">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G36" s="33" t="s">
         <v>19</v>
@@ -3081,7 +3081,7 @@
       <c r="M36" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N36" s="64" t="s">
+      <c r="N36" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q36">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G37" s="33" t="s">
         <v>19</v>
@@ -3123,7 +3123,7 @@
       <c r="M37" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N37" s="64" t="s">
+      <c r="N37" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q37">
@@ -3147,7 +3147,7 @@
         <v>146</v>
       </c>
       <c r="F38" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G38" s="33" t="s">
         <v>19</v>
@@ -3167,7 +3167,7 @@
       <c r="M38" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N38" s="64" t="s">
+      <c r="N38" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q38">
@@ -3191,7 +3191,7 @@
         <v>146</v>
       </c>
       <c r="F39" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G39" s="33" t="s">
         <v>19</v>
@@ -3211,7 +3211,7 @@
       <c r="M39" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N39" s="64" t="s">
+      <c r="N39" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q39">
@@ -3235,7 +3235,7 @@
         <v>146</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G40" s="33" t="s">
         <v>19</v>
@@ -3255,7 +3255,7 @@
       <c r="M40" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N40" s="64" t="s">
+      <c r="N40" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q40">
@@ -3279,7 +3279,7 @@
         <v>146</v>
       </c>
       <c r="F41" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G41" s="33" t="s">
         <v>19</v>
@@ -3299,7 +3299,7 @@
       <c r="M41" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N41" s="64" t="s">
+      <c r="N41" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q41">
@@ -3323,7 +3323,7 @@
         <v>146</v>
       </c>
       <c r="F42" s="33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G42" s="33" t="s">
         <v>19</v>
@@ -3343,7 +3343,7 @@
       <c r="M42" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N42" s="64" t="s">
+      <c r="N42" s="38" t="s">
         <v>147</v>
       </c>
       <c r="Q42">
@@ -3373,7 +3373,7 @@
       <c r="I43" s="35">
         <v>298</v>
       </c>
-      <c r="J43" s="65">
+      <c r="J43" s="39">
         <v>50</v>
       </c>
       <c r="K43" s="32"/>
@@ -3383,7 +3383,7 @@
       <c r="M43" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N43" s="64" t="s">
+      <c r="N43" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3410,7 +3410,7 @@
       <c r="I44" s="35">
         <v>298</v>
       </c>
-      <c r="J44" s="65">
+      <c r="J44" s="39">
         <v>14.9</v>
       </c>
       <c r="K44" s="32"/>
@@ -3420,7 +3420,7 @@
       <c r="M44" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N44" s="64" t="s">
+      <c r="N44" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3447,7 +3447,7 @@
       <c r="I45" s="35">
         <v>298</v>
       </c>
-      <c r="J45" s="65">
+      <c r="J45" s="39">
         <v>14.2</v>
       </c>
       <c r="K45" s="32"/>
@@ -3457,7 +3457,7 @@
       <c r="M45" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N45" s="64" t="s">
+      <c r="N45" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3484,7 +3484,7 @@
       <c r="I46" s="35">
         <v>298</v>
       </c>
-      <c r="J46" s="65">
+      <c r="J46" s="39">
         <v>12.1</v>
       </c>
       <c r="K46" s="32"/>
@@ -3494,7 +3494,7 @@
       <c r="M46" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N46" s="64" t="s">
+      <c r="N46" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3521,7 +3521,7 @@
       <c r="I47" s="35">
         <v>298</v>
       </c>
-      <c r="J47" s="65">
+      <c r="J47" s="39">
         <v>9.1999999999999993</v>
       </c>
       <c r="K47" s="32"/>
@@ -3531,7 +3531,7 @@
       <c r="M47" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N47" s="64" t="s">
+      <c r="N47" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3560,7 +3560,7 @@
       <c r="I48" s="35">
         <v>298</v>
       </c>
-      <c r="J48" s="65">
+      <c r="J48" s="39">
         <v>3.5</v>
       </c>
       <c r="K48" s="32"/>
@@ -3570,7 +3570,7 @@
       <c r="M48" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N48" s="64" t="s">
+      <c r="N48" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3599,7 +3599,7 @@
       <c r="I49" s="35">
         <v>298</v>
       </c>
-      <c r="J49" s="65">
+      <c r="J49" s="39">
         <v>6.2</v>
       </c>
       <c r="K49" s="32"/>
@@ -3609,7 +3609,7 @@
       <c r="M49" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N49" s="64" t="s">
+      <c r="N49" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3638,7 +3638,7 @@
       <c r="I50" s="35">
         <v>298</v>
       </c>
-      <c r="J50" s="65">
+      <c r="J50" s="39">
         <v>7</v>
       </c>
       <c r="K50" s="32"/>
@@ -3648,7 +3648,7 @@
       <c r="M50" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N50" s="64" t="s">
+      <c r="N50" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3677,7 +3677,7 @@
       <c r="I51" s="35">
         <v>298</v>
       </c>
-      <c r="J51" s="65">
+      <c r="J51" s="39">
         <v>8.1999999999999993</v>
       </c>
       <c r="K51" s="32"/>
@@ -3687,7 +3687,7 @@
       <c r="M51" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N51" s="64" t="s">
+      <c r="N51" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3716,7 +3716,7 @@
       <c r="I52" s="35">
         <v>298</v>
       </c>
-      <c r="J52" s="65">
+      <c r="J52" s="39">
         <v>8.5</v>
       </c>
       <c r="K52" s="32"/>
@@ -3726,7 +3726,7 @@
       <c r="M52" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N52" s="64" t="s">
+      <c r="N52" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3765,7 +3765,7 @@
       <c r="M53" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N53" s="64" t="s">
+      <c r="N53" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P53">
@@ -3807,7 +3807,7 @@
       <c r="M54" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N54" s="64" t="s">
+      <c r="N54" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P54">
@@ -3849,7 +3849,7 @@
       <c r="M55" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N55" s="64" t="s">
+      <c r="N55" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P55">
@@ -3891,7 +3891,7 @@
       <c r="M56" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N56" s="64" t="s">
+      <c r="N56" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P56">
@@ -3933,7 +3933,7 @@
       <c r="M57" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N57" s="64" t="s">
+      <c r="N57" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P57">
@@ -3977,7 +3977,7 @@
       <c r="M58" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N58" s="64" t="s">
+      <c r="N58" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P58">
@@ -4021,7 +4021,7 @@
       <c r="M59" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N59" s="64" t="s">
+      <c r="N59" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P59">
@@ -4065,7 +4065,7 @@
       <c r="M60" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N60" s="64" t="s">
+      <c r="N60" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P60">
@@ -4109,7 +4109,7 @@
       <c r="M61" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N61" s="64" t="s">
+      <c r="N61" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P61">
@@ -4153,7 +4153,7 @@
       <c r="M62" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N62" s="64" t="s">
+      <c r="N62" s="38" t="s">
         <v>147</v>
       </c>
       <c r="P62">
@@ -4175,7 +4175,7 @@
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G63" s="33" t="s">
         <v>19</v>
@@ -4185,16 +4185,16 @@
         <v>293</v>
       </c>
       <c r="J63" s="32">
-        <v>9.5749999999999993</v>
+        <v>9575</v>
       </c>
       <c r="K63" s="32"/>
       <c r="L63" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M63" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N63" s="64" t="s">
+      <c r="N63" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G64" s="33" t="s">
         <v>19</v>
@@ -4223,16 +4223,16 @@
         <v>293</v>
       </c>
       <c r="J64" s="32">
-        <v>10.324</v>
+        <v>10324</v>
       </c>
       <c r="K64" s="32"/>
       <c r="L64" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M64" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N64" s="64" t="s">
+      <c r="N64" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G65" s="33" t="s">
         <v>19</v>
@@ -4261,16 +4261,16 @@
         <v>293</v>
       </c>
       <c r="J65" s="32">
-        <v>10.32</v>
+        <v>10320</v>
       </c>
       <c r="K65" s="32"/>
       <c r="L65" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M65" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N65" s="64" t="s">
+      <c r="N65" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G66" s="33" t="s">
         <v>19</v>
@@ -4299,16 +4299,16 @@
         <v>293</v>
       </c>
       <c r="J66" s="32">
-        <v>10.194000000000001</v>
+        <v>10194</v>
       </c>
       <c r="K66" s="32"/>
       <c r="L66" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M66" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N66" s="64" t="s">
+      <c r="N66" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4327,7 +4327,7 @@
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G67" s="33" t="s">
         <v>19</v>
@@ -4337,16 +4337,16 @@
         <v>293</v>
       </c>
       <c r="J67" s="32">
-        <v>10.055999999999999</v>
+        <v>10056</v>
       </c>
       <c r="K67" s="32"/>
       <c r="L67" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M67" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N67" s="64" t="s">
+      <c r="N67" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4367,7 +4367,7 @@
         <v>146</v>
       </c>
       <c r="F68" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G68" s="33" t="s">
         <v>19</v>
@@ -4377,16 +4377,16 @@
         <v>293</v>
       </c>
       <c r="J68" s="32">
-        <v>9.58</v>
+        <v>9580</v>
       </c>
       <c r="K68" s="32"/>
       <c r="L68" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M68" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N68" s="64" t="s">
+      <c r="N68" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4407,7 +4407,7 @@
         <v>146</v>
       </c>
       <c r="F69" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G69" s="33" t="s">
         <v>19</v>
@@ -4417,16 +4417,16 @@
         <v>293</v>
       </c>
       <c r="J69" s="32">
-        <v>9.952</v>
+        <v>9952</v>
       </c>
       <c r="K69" s="32"/>
       <c r="L69" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M69" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N69" s="64" t="s">
+      <c r="N69" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4447,7 +4447,7 @@
         <v>146</v>
       </c>
       <c r="F70" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G70" s="33" t="s">
         <v>19</v>
@@ -4457,16 +4457,16 @@
         <v>293</v>
       </c>
       <c r="J70" s="32">
-        <v>9.7129999999999992</v>
+        <v>9713</v>
       </c>
       <c r="K70" s="32"/>
       <c r="L70" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M70" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N70" s="64" t="s">
+      <c r="N70" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4487,7 +4487,7 @@
         <v>146</v>
       </c>
       <c r="F71" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G71" s="33" t="s">
         <v>19</v>
@@ -4497,16 +4497,16 @@
         <v>293</v>
       </c>
       <c r="J71" s="32">
-        <v>9.6530000000000005</v>
+        <v>9653</v>
       </c>
       <c r="K71" s="32"/>
       <c r="L71" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M71" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N71" s="64" t="s">
+      <c r="N71" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4527,7 +4527,7 @@
         <v>146</v>
       </c>
       <c r="F72" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G72" s="33" t="s">
         <v>19</v>
@@ -4537,16 +4537,16 @@
         <v>293</v>
       </c>
       <c r="J72" s="32">
-        <v>9.4130000000000003</v>
+        <v>9413</v>
       </c>
       <c r="K72" s="32"/>
       <c r="L72" s="20" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="M72" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="N72" s="64" t="s">
+      <c r="N72" s="38" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4555,16 +4555,16 @@
         <v>67</v>
       </c>
       <c r="B73" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C73" s="33" t="s">
         <v>125</v>
       </c>
       <c r="D73" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E73" s="20" t="s">
         <v>155</v>
-      </c>
-      <c r="E73" s="20" t="s">
-        <v>156</v>
       </c>
       <c r="F73" s="33" t="s">
         <v>133</v>
@@ -4577,7 +4577,7 @@
         <v>298</v>
       </c>
       <c r="J73" s="32">
-        <f t="shared" ref="J73:J76" si="3">Q73*1000000</f>
+        <f>Q73*1000000</f>
         <v>997000000</v>
       </c>
       <c r="K73" s="32"/>
@@ -4585,10 +4585,10 @@
         <v>42</v>
       </c>
       <c r="M73" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N73" s="64" t="s">
-        <v>158</v>
+        <v>161</v>
+      </c>
+      <c r="N73" s="38" t="s">
+        <v>157</v>
       </c>
       <c r="Q73">
         <v>997</v>
@@ -4599,16 +4599,16 @@
         <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C74" s="33" t="s">
         <v>125</v>
       </c>
       <c r="D74" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F74" s="33" t="s">
         <v>133</v>
@@ -4621,7 +4621,7 @@
         <v>298</v>
       </c>
       <c r="J74" s="32">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J73:J76" si="3">Q74*1000000</f>
         <v>841000000</v>
       </c>
       <c r="K74" s="32"/>
@@ -4629,10 +4629,10 @@
         <v>42</v>
       </c>
       <c r="M74" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N74" s="64" t="s">
-        <v>158</v>
+        <v>161</v>
+      </c>
+      <c r="N74" s="38" t="s">
+        <v>157</v>
       </c>
       <c r="Q74">
         <v>841</v>
@@ -4643,19 +4643,19 @@
         <v>69</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C75" s="33" t="s">
         <v>125</v>
       </c>
       <c r="D75" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E75" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="E75" s="20" t="s">
-        <v>156</v>
-      </c>
       <c r="F75" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G75" s="33" t="s">
         <v>19</v>
@@ -4673,10 +4673,10 @@
         <v>42</v>
       </c>
       <c r="M75" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N75" s="64" t="s">
-        <v>158</v>
+        <v>161</v>
+      </c>
+      <c r="N75" s="38" t="s">
+        <v>157</v>
       </c>
       <c r="Q75">
         <v>1043</v>
@@ -4687,19 +4687,19 @@
         <v>70</v>
       </c>
       <c r="B76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C76" s="33" t="s">
         <v>125</v>
       </c>
       <c r="D76" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F76" s="33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G76" s="33" t="s">
         <v>19</v>
@@ -4717,10 +4717,10 @@
         <v>42</v>
       </c>
       <c r="M76" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N76" s="64" t="s">
-        <v>158</v>
+        <v>161</v>
+      </c>
+      <c r="N76" s="38" t="s">
+        <v>157</v>
       </c>
       <c r="Q76">
         <v>857</v>
@@ -4731,16 +4731,16 @@
         <v>71</v>
       </c>
       <c r="B77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C77" s="33" t="s">
         <v>125</v>
       </c>
       <c r="D77" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="E77" s="20" t="s">
         <v>155</v>
-      </c>
-      <c r="E77" s="20" t="s">
-        <v>156</v>
       </c>
       <c r="F77" s="33" t="s">
         <v>136</v>
@@ -4760,10 +4760,10 @@
         <v>63</v>
       </c>
       <c r="M77" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N77" s="64" t="s">
-        <v>158</v>
+        <v>161</v>
+      </c>
+      <c r="N77" s="38" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.2">
@@ -4771,16 +4771,16 @@
         <v>72</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C78" s="33" t="s">
         <v>125</v>
       </c>
       <c r="D78" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E78" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F78" s="33" t="s">
         <v>136</v>
@@ -4800,10 +4800,10 @@
         <v>63</v>
       </c>
       <c r="M78" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N78" s="64" t="s">
-        <v>158</v>
+        <v>161</v>
+      </c>
+      <c r="N78" s="38" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.2">
@@ -4811,7 +4811,7 @@
         <v>67</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C79" s="33" t="s">
         <v>125</v>
@@ -4820,7 +4820,7 @@
         <v>65</v>
       </c>
       <c r="E79" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F79" s="33" t="s">
         <v>133</v>
@@ -4841,10 +4841,10 @@
         <v>42</v>
       </c>
       <c r="M79" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N79" s="64" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="N79" s="38" t="s">
+        <v>159</v>
       </c>
       <c r="Q79">
         <v>850</v>
@@ -4855,7 +4855,7 @@
         <v>68</v>
       </c>
       <c r="B80" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C80" s="33" t="s">
         <v>125</v>
@@ -4864,7 +4864,7 @@
         <v>65</v>
       </c>
       <c r="E80" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F80" s="33" t="s">
         <v>133</v>
@@ -4885,10 +4885,10 @@
         <v>42</v>
       </c>
       <c r="M80" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="N80" s="64" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="N80" s="38" t="s">
+        <v>159</v>
       </c>
       <c r="Q80">
         <v>721</v>
@@ -4899,7 +4899,7 @@
         <v>69</v>
       </c>
       <c r="B81" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C81" s="33" t="s">
         <v>125</v>
@@ -4908,7 +4908,7 @@
         <v>65</v>
       </c>
       <c r="E81" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F81" s="33" t="s">
         <v>133</v>
@@ -4929,10 +4929,10 @@
         <v>42</v>
       </c>
       <c r="M81" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N81" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N81" s="64" t="s">
-        <v>163</v>
       </c>
       <c r="Q81">
         <v>668</v>
@@ -4943,7 +4943,7 @@
         <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C82" s="33" t="s">
         <v>125</v>
@@ -4952,7 +4952,7 @@
         <v>65</v>
       </c>
       <c r="E82" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F82" s="33" t="s">
         <v>136</v>
@@ -4972,10 +4972,10 @@
         <v>63</v>
       </c>
       <c r="M82" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N82" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N82" s="64" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.2">
@@ -4983,7 +4983,7 @@
         <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C83" s="33" t="s">
         <v>125</v>
@@ -4992,7 +4992,7 @@
         <v>65</v>
       </c>
       <c r="E83" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F83" s="33" t="s">
         <v>136</v>
@@ -5012,10 +5012,10 @@
         <v>63</v>
       </c>
       <c r="M83" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N83" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N83" s="64" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.2">
@@ -5023,7 +5023,7 @@
         <v>72</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C84" s="33" t="s">
         <v>125</v>
@@ -5032,7 +5032,7 @@
         <v>65</v>
       </c>
       <c r="E84" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F84" s="33" t="s">
         <v>136</v>
@@ -5052,10 +5052,10 @@
         <v>63</v>
       </c>
       <c r="M84" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N84" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N84" s="64" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.2">
@@ -5063,7 +5063,7 @@
         <v>73</v>
       </c>
       <c r="B85" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C85" s="33" t="s">
         <v>125</v>
@@ -5072,7 +5072,7 @@
         <v>65</v>
       </c>
       <c r="E85" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F85" s="33" t="s">
         <v>66</v>
@@ -5096,10 +5096,10 @@
         <v>42</v>
       </c>
       <c r="M85" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N85" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N85" s="64" t="s">
-        <v>163</v>
       </c>
       <c r="P85">
         <v>311</v>
@@ -5113,7 +5113,7 @@
         <v>74</v>
       </c>
       <c r="B86" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C86" s="33" t="s">
         <v>125</v>
@@ -5122,7 +5122,7 @@
         <v>65</v>
       </c>
       <c r="E86" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F86" s="33" t="s">
         <v>133</v>
@@ -5143,10 +5143,10 @@
         <v>42</v>
       </c>
       <c r="M86" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N86" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N86" s="64" t="s">
-        <v>163</v>
       </c>
       <c r="Q86">
         <v>848</v>
@@ -5157,7 +5157,7 @@
         <v>75</v>
       </c>
       <c r="B87" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C87" s="33" t="s">
         <v>125</v>
@@ -5166,7 +5166,7 @@
         <v>65</v>
       </c>
       <c r="E87" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F87" s="33" t="s">
         <v>133</v>
@@ -5187,10 +5187,10 @@
         <v>42</v>
       </c>
       <c r="M87" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N87" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N87" s="64" t="s">
-        <v>163</v>
       </c>
       <c r="Q87">
         <v>635</v>
@@ -5201,7 +5201,7 @@
         <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C88" s="33" t="s">
         <v>125</v>
@@ -5210,7 +5210,7 @@
         <v>65</v>
       </c>
       <c r="E88" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F88" s="33" t="s">
         <v>133</v>
@@ -5231,10 +5231,10 @@
         <v>42</v>
       </c>
       <c r="M88" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N88" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N88" s="64" t="s">
-        <v>163</v>
       </c>
       <c r="Q88">
         <v>583</v>
@@ -5245,7 +5245,7 @@
         <v>77</v>
       </c>
       <c r="B89" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C89" s="33" t="s">
         <v>125</v>
@@ -5254,7 +5254,7 @@
         <v>65</v>
       </c>
       <c r="E89" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F89" s="33" t="s">
         <v>136</v>
@@ -5274,10 +5274,10 @@
         <v>63</v>
       </c>
       <c r="M89" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N89" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N89" s="64" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
@@ -5285,7 +5285,7 @@
         <v>78</v>
       </c>
       <c r="B90" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C90" s="33" t="s">
         <v>125</v>
@@ -5294,7 +5294,7 @@
         <v>65</v>
       </c>
       <c r="E90" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F90" s="33" t="s">
         <v>136</v>
@@ -5314,10 +5314,10 @@
         <v>63</v>
       </c>
       <c r="M90" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N90" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N90" s="64" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
@@ -5325,7 +5325,7 @@
         <v>79</v>
       </c>
       <c r="B91" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C91" s="33" t="s">
         <v>125</v>
@@ -5334,7 +5334,7 @@
         <v>65</v>
       </c>
       <c r="E91" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F91" s="33" t="s">
         <v>136</v>
@@ -5354,10 +5354,10 @@
         <v>63</v>
       </c>
       <c r="M91" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N91" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N91" s="64" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
@@ -5365,7 +5365,7 @@
         <v>80</v>
       </c>
       <c r="B92" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C92" s="33" t="s">
         <v>125</v>
@@ -5374,7 +5374,7 @@
         <v>65</v>
       </c>
       <c r="E92" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F92" s="33" t="s">
         <v>66</v>
@@ -5398,10 +5398,10 @@
         <v>42</v>
       </c>
       <c r="M92" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="N92" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="N92" s="64" t="s">
-        <v>163</v>
       </c>
       <c r="P92">
         <v>314</v>
@@ -10299,11 +10299,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10318,6 +10313,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
- fix literature error in `10.1016/j.jallcom.2022.166593`
</commit_message>
<xml_diff>
--- a/Compilation_HardnessAndDuctility.xlsx
+++ b/Compilation_HardnessAndDuctility.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-amkrajewski/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A925131-B2A3-B64C-A5B1-8FAFA12C6C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFE864A-5956-2141-8CB4-40DEFB67507A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="33760" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1293,33 +1293,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1369,6 +1342,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1654,8 +1654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1691,19 +1691,19 @@
       <c r="B2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1713,17 +1713,17 @@
       <c r="B3" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="52"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
       <c r="O3" s="25"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1741,43 +1741,43 @@
       <c r="B5" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="46" t="s">
+      <c r="I5" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="46" t="s">
+      <c r="L5" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="46" t="s">
+      <c r="M5" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="46" t="s">
+      <c r="N5" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="58" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1788,19 +1788,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="41"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="59"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1845,7 +1845,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="42"/>
+      <c r="O7" s="60"/>
       <c r="P7" s="31" t="s">
         <v>126</v>
       </c>
@@ -1858,35 +1858,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60" t="s">
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="63" t="s">
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="64"/>
+      <c r="N8" s="55"/>
       <c r="O8" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="P8" s="43" t="s">
+      <c r="P8" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="45"/>
+      <c r="Q8" s="62"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="62"/>
+      <c r="T8" s="63"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -4185,7 +4185,7 @@
         <v>293</v>
       </c>
       <c r="J63" s="32">
-        <v>9575</v>
+        <v>10575</v>
       </c>
       <c r="K63" s="32"/>
       <c r="L63" s="20" t="s">
@@ -4377,7 +4377,7 @@
         <v>293</v>
       </c>
       <c r="J68" s="32">
-        <v>9580</v>
+        <v>10580</v>
       </c>
       <c r="K68" s="32"/>
       <c r="L68" s="20" t="s">
@@ -4621,7 +4621,7 @@
         <v>298</v>
       </c>
       <c r="J74" s="32">
-        <f t="shared" ref="J73:J76" si="3">Q74*1000000</f>
+        <f t="shared" ref="J74:J76" si="3">Q74*1000000</f>
         <v>841000000</v>
       </c>
       <c r="K74" s="32"/>
@@ -10299,6 +10299,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10313,11 +10318,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>